<commit_message>
Update project dependencies and data files
Updated the SDK version in project configuration to Python 3.11 (kaggle). Also, revised three data files: CORTE_SAP.xlsx, saved_df_2024_10.csv, and tiempo_final.xlsx to include the latest data.
</commit_message>
<xml_diff>
--- a/data/tiempo_final.xlsx
+++ b/data/tiempo_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="836">
   <si>
     <t>timestamp</t>
   </si>
@@ -1573,6 +1573,12 @@
     <t>L_04021.NC</t>
   </si>
   <si>
+    <t>2024-10-10 12:09:22</t>
+  </si>
+  <si>
+    <t>L_0416.slp</t>
+  </si>
+  <si>
     <t>2024-09-25 14:49:38</t>
   </si>
   <si>
@@ -1651,6 +1657,12 @@
     <t>L_04627.NC</t>
   </si>
   <si>
+    <t>2024-10-15 00:49:53</t>
+  </si>
+  <si>
+    <t>L_04628.NC</t>
+  </si>
+  <si>
     <t>2024-10-15 02:39:53</t>
   </si>
   <si>
@@ -1711,18 +1723,90 @@
     <t>L_04638.NC</t>
   </si>
   <si>
+    <t>2024-10-16 14:30:52</t>
+  </si>
+  <si>
+    <t>L_04639.NC</t>
+  </si>
+  <si>
+    <t>2024-10-14 09:47:25</t>
+  </si>
+  <si>
+    <t>L_04640.NC</t>
+  </si>
+  <si>
+    <t>2024-10-17 22:55:16</t>
+  </si>
+  <si>
+    <t>L_04641.NC</t>
+  </si>
+  <si>
+    <t>2024-10-17 21:57:32</t>
+  </si>
+  <si>
+    <t>L_04642.NC</t>
+  </si>
+  <si>
+    <t>2024-10-17 23:02:37</t>
+  </si>
+  <si>
+    <t>L_04643.NC</t>
+  </si>
+  <si>
+    <t>2024-10-17 22:48:17</t>
+  </si>
+  <si>
+    <t>L_04644.NC</t>
+  </si>
+  <si>
+    <t>2024-10-17 23:26:53</t>
+  </si>
+  <si>
+    <t>L_04645.NC</t>
+  </si>
+  <si>
+    <t>2024-10-16 14:21:12</t>
+  </si>
+  <si>
+    <t>L_04646.NC</t>
+  </si>
+  <si>
+    <t>2024-10-16 10:58:09</t>
+  </si>
+  <si>
+    <t>L_04647.NC</t>
+  </si>
+  <si>
     <t>2024-10-15 08:28:14</t>
   </si>
   <si>
     <t>L_04648.NC</t>
   </si>
   <si>
+    <t>2024-10-16 10:48:43</t>
+  </si>
+  <si>
+    <t>L_04649.NC</t>
+  </si>
+  <si>
     <t>2024-10-15 11:29:15</t>
   </si>
   <si>
     <t>L_04650.NC</t>
   </si>
   <si>
+    <t>2024-10-16 10:40:06</t>
+  </si>
+  <si>
+    <t>L_04651.NC</t>
+  </si>
+  <si>
+    <t>2024-10-17 22:12:25</t>
+  </si>
+  <si>
+    <t>L_04652.NC</t>
+  </si>
+  <si>
     <t>2024-10-15 08:15:18</t>
   </si>
   <si>
@@ -1753,6 +1837,18 @@
     <t>L_04660.NC</t>
   </si>
   <si>
+    <t>2024-10-18 01:36:57</t>
+  </si>
+  <si>
+    <t>L_04661.NC</t>
+  </si>
+  <si>
+    <t>2024-10-16 11:46:51</t>
+  </si>
+  <si>
+    <t>L_04662.NC</t>
+  </si>
+  <si>
     <t>2024-10-15 04:47:01</t>
   </si>
   <si>
@@ -1771,24 +1867,72 @@
     <t>L_04670.NC</t>
   </si>
   <si>
+    <t>2024-10-16 11:58:42</t>
+  </si>
+  <si>
+    <t>L_04671.NC</t>
+  </si>
+  <si>
     <t>2024-10-15 03:17:38</t>
   </si>
   <si>
     <t>L_04672.NC</t>
   </si>
   <si>
+    <t>2024-10-16 14:38:35</t>
+  </si>
+  <si>
+    <t>L_04673.NC</t>
+  </si>
+  <si>
     <t>2024-10-14 10:06:27</t>
   </si>
   <si>
     <t>L_04674.NC</t>
   </si>
   <si>
+    <t>2024-10-16 12:07:08</t>
+  </si>
+  <si>
+    <t>L_04675.NC</t>
+  </si>
+  <si>
     <t>2024-10-14 12:49:53</t>
   </si>
   <si>
     <t>L_04676.NC</t>
   </si>
   <si>
+    <t>2024-10-17 23:34:10</t>
+  </si>
+  <si>
+    <t>L_04677.NC</t>
+  </si>
+  <si>
+    <t>2024-10-17 23:41:48</t>
+  </si>
+  <si>
+    <t>L_04678.NC</t>
+  </si>
+  <si>
+    <t>2024-10-18 01:25:10</t>
+  </si>
+  <si>
+    <t>L_04679.NC</t>
+  </si>
+  <si>
+    <t>2024-10-18 01:17:36</t>
+  </si>
+  <si>
+    <t>L_04680.NC</t>
+  </si>
+  <si>
+    <t>2024-10-18 02:04:17</t>
+  </si>
+  <si>
+    <t>L_04681.NC</t>
+  </si>
+  <si>
     <t>2024-10-11 02:45:28</t>
   </si>
   <si>
@@ -2117,6 +2261,180 @@
   </si>
   <si>
     <t>L_05119.NC</t>
+  </si>
+  <si>
+    <t>2024-10-16 05:44:41</t>
+  </si>
+  <si>
+    <t>L_05168.NC</t>
+  </si>
+  <si>
+    <t>2024-10-18 02:51:38</t>
+  </si>
+  <si>
+    <t>L_05176.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 08:51:14</t>
+  </si>
+  <si>
+    <t>L_05177.NC</t>
+  </si>
+  <si>
+    <t>2024-10-18 03:29:56</t>
+  </si>
+  <si>
+    <t>L_05178.NC</t>
+  </si>
+  <si>
+    <t>2024-10-15 22:35:46</t>
+  </si>
+  <si>
+    <t>L_05208.NC</t>
+  </si>
+  <si>
+    <t>2024-10-15 15:02:49</t>
+  </si>
+  <si>
+    <t>L_05209.NC</t>
+  </si>
+  <si>
+    <t>2024-10-15 12:45:01</t>
+  </si>
+  <si>
+    <t>L_05210.NC</t>
+  </si>
+  <si>
+    <t>2024-10-15 11:41:01</t>
+  </si>
+  <si>
+    <t>L_05211.NC</t>
+  </si>
+  <si>
+    <t>2024-10-16 16:21:12</t>
+  </si>
+  <si>
+    <t>L_05249.NC</t>
+  </si>
+  <si>
+    <t>2024-10-18 10:07:35</t>
+  </si>
+  <si>
+    <t>L_05257.NC</t>
+  </si>
+  <si>
+    <t>2024-10-18 02:44:37</t>
+  </si>
+  <si>
+    <t>L_05258.slp</t>
+  </si>
+  <si>
+    <t>2024-10-18 08:29:53</t>
+  </si>
+  <si>
+    <t>L_05259.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 08:30:14</t>
+  </si>
+  <si>
+    <t>L_05260.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 15:45:27</t>
+  </si>
+  <si>
+    <t>L_05297.NC</t>
+  </si>
+  <si>
+    <t>2024-10-22 10:57:52</t>
+  </si>
+  <si>
+    <t>L_05298.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 09:51:13</t>
+  </si>
+  <si>
+    <t>L_05304.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 11:29:50</t>
+  </si>
+  <si>
+    <t>L_05305.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 10:33:12</t>
+  </si>
+  <si>
+    <t>L_05306.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 08:56:00</t>
+  </si>
+  <si>
+    <t>L_05307.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 12:53:54</t>
+  </si>
+  <si>
+    <t>L_05308.NC</t>
+  </si>
+  <si>
+    <t>2024-10-21 13:25:35</t>
+  </si>
+  <si>
+    <t>L_05309.NC</t>
+  </si>
+  <si>
+    <t>2024-10-22 14:28:07</t>
+  </si>
+  <si>
+    <t>L_05466.NC</t>
+  </si>
+  <si>
+    <t>2024-10-22 14:29:17</t>
+  </si>
+  <si>
+    <t>L_05467.NC</t>
+  </si>
+  <si>
+    <t>2024-10-23 11:04:12</t>
+  </si>
+  <si>
+    <t>L_05566.NC</t>
+  </si>
+  <si>
+    <t>2024-10-23 13:57:18</t>
+  </si>
+  <si>
+    <t>L_05567.NC</t>
+  </si>
+  <si>
+    <t>2024-10-23 12:20:53</t>
+  </si>
+  <si>
+    <t>L_05569.NC</t>
+  </si>
+  <si>
+    <t>2024-10-23 14:29:51</t>
+  </si>
+  <si>
+    <t>L_05570.NC</t>
+  </si>
+  <si>
+    <t>2024-10-23 09:09:52</t>
+  </si>
+  <si>
+    <t>L_05629.NC</t>
+  </si>
+  <si>
+    <t>2024-10-23 16:33:57</t>
+  </si>
+  <si>
+    <t>L_05682.NC</t>
   </si>
   <si>
     <t>2024-06-12 08:57:56</t>
@@ -2306,7 +2624,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -2316,16 +2634,19 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2497,9 +2818,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -2579,7 +2900,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2607,10 +2928,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2866,9 +3187,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
+              <a:alpha val="38000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -3156,7 +3477,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3184,10 +3505,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3438,15 +3759,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F363"/>
+  <dimension ref="A1:F416"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3516" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.9297" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.2344" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.2109" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5078" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8618,13 +8942,13 @@
         <v>521</v>
       </c>
       <c r="C259" s="6">
-        <v>29.32</v>
+        <v>4</v>
       </c>
       <c r="D259" s="6">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="E259" s="6">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F259" s="6">
         <v>1</v>
@@ -8638,13 +8962,13 @@
         <v>523</v>
       </c>
       <c r="C260" s="6">
-        <v>496</v>
+        <v>29.32</v>
       </c>
       <c r="D260" s="6">
-        <v>939</v>
+        <v>86</v>
       </c>
       <c r="E260" s="6">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F260" s="6">
         <v>1</v>
@@ -8658,13 +8982,13 @@
         <v>525</v>
       </c>
       <c r="C261" s="6">
-        <v>4</v>
+        <v>496</v>
       </c>
       <c r="D261" s="6">
-        <v>26</v>
+        <v>939</v>
       </c>
       <c r="E261" s="6">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F261" s="6">
         <v>1</v>
@@ -8918,7 +9242,7 @@
         <v>551</v>
       </c>
       <c r="C274" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D274" s="6">
         <v>26</v>
@@ -8938,10 +9262,10 @@
         <v>553</v>
       </c>
       <c r="C275" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D275" s="6">
-        <v>25.4</v>
+        <v>26</v>
       </c>
       <c r="E275" s="6">
         <v>3</v>
@@ -8958,7 +9282,7 @@
         <v>555</v>
       </c>
       <c r="C276" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D276" s="6">
         <v>26</v>
@@ -9001,7 +9325,7 @@
         <v>5</v>
       </c>
       <c r="D278" s="6">
-        <v>25.4</v>
+        <v>26</v>
       </c>
       <c r="E278" s="6">
         <v>3</v>
@@ -9018,10 +9342,10 @@
         <v>561</v>
       </c>
       <c r="C279" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D279" s="6">
-        <v>26</v>
+        <v>25.4</v>
       </c>
       <c r="E279" s="6">
         <v>3</v>
@@ -9041,7 +9365,7 @@
         <v>5</v>
       </c>
       <c r="D280" s="6">
-        <v>26</v>
+        <v>25.4</v>
       </c>
       <c r="E280" s="6">
         <v>3</v>
@@ -9081,7 +9405,7 @@
         <v>5</v>
       </c>
       <c r="D282" s="6">
-        <v>25.5</v>
+        <v>26</v>
       </c>
       <c r="E282" s="6">
         <v>3</v>
@@ -9118,10 +9442,10 @@
         <v>571</v>
       </c>
       <c r="C284" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D284" s="6">
-        <v>44</v>
+        <v>25.4</v>
       </c>
       <c r="E284" s="6">
         <v>3</v>
@@ -9138,10 +9462,10 @@
         <v>573</v>
       </c>
       <c r="C285" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D285" s="6">
-        <v>44</v>
+        <v>25.4</v>
       </c>
       <c r="E285" s="6">
         <v>3</v>
@@ -9158,10 +9482,10 @@
         <v>575</v>
       </c>
       <c r="C286" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D286" s="6">
-        <v>44</v>
+        <v>25.4</v>
       </c>
       <c r="E286" s="6">
         <v>3</v>
@@ -9178,10 +9502,10 @@
         <v>577</v>
       </c>
       <c r="C287" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D287" s="6">
-        <v>44</v>
+        <v>25.4</v>
       </c>
       <c r="E287" s="6">
         <v>3</v>
@@ -9198,10 +9522,10 @@
         <v>579</v>
       </c>
       <c r="C288" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D288" s="6">
-        <v>44</v>
+        <v>25.4</v>
       </c>
       <c r="E288" s="6">
         <v>3</v>
@@ -9218,10 +9542,10 @@
         <v>581</v>
       </c>
       <c r="C289" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D289" s="6">
-        <v>44</v>
+        <v>25.4</v>
       </c>
       <c r="E289" s="6">
         <v>3</v>
@@ -9238,10 +9562,10 @@
         <v>583</v>
       </c>
       <c r="C290" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D290" s="6">
-        <v>40</v>
+        <v>25.4</v>
       </c>
       <c r="E290" s="6">
         <v>3</v>
@@ -9258,10 +9582,10 @@
         <v>585</v>
       </c>
       <c r="C291" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D291" s="6">
-        <v>31.4</v>
+        <v>25.4</v>
       </c>
       <c r="E291" s="6">
         <v>3</v>
@@ -9278,10 +9602,10 @@
         <v>587</v>
       </c>
       <c r="C292" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D292" s="6">
-        <v>31.3</v>
+        <v>25.4</v>
       </c>
       <c r="E292" s="6">
         <v>3</v>
@@ -9298,10 +9622,10 @@
         <v>589</v>
       </c>
       <c r="C293" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D293" s="6">
-        <v>31.3</v>
+        <v>25.5</v>
       </c>
       <c r="E293" s="6">
         <v>3</v>
@@ -9318,10 +9642,10 @@
         <v>591</v>
       </c>
       <c r="C294" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D294" s="6">
-        <v>31.3</v>
+        <v>25.4</v>
       </c>
       <c r="E294" s="6">
         <v>3</v>
@@ -9338,13 +9662,13 @@
         <v>593</v>
       </c>
       <c r="C295" s="6">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="D295" s="6">
-        <v>428.3</v>
+        <v>26</v>
       </c>
       <c r="E295" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F295" s="6">
         <v>1</v>
@@ -9358,13 +9682,13 @@
         <v>595</v>
       </c>
       <c r="C296" s="6">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="D296" s="6">
-        <v>222.6</v>
+        <v>25.4</v>
       </c>
       <c r="E296" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F296" s="6">
         <v>1</v>
@@ -9378,13 +9702,13 @@
         <v>597</v>
       </c>
       <c r="C297" s="6">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="D297" s="6">
-        <v>71.5</v>
+        <v>25.4</v>
       </c>
       <c r="E297" s="6">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F297" s="6">
         <v>1</v>
@@ -9398,13 +9722,13 @@
         <v>599</v>
       </c>
       <c r="C298" s="6">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D298" s="6">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E298" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F298" s="6">
         <v>1</v>
@@ -9418,13 +9742,13 @@
         <v>601</v>
       </c>
       <c r="C299" s="6">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D299" s="6">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E299" s="6">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F299" s="6">
         <v>1</v>
@@ -9438,13 +9762,13 @@
         <v>603</v>
       </c>
       <c r="C300" s="6">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D300" s="6">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="E300" s="6">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F300" s="6">
         <v>1</v>
@@ -9458,13 +9782,13 @@
         <v>605</v>
       </c>
       <c r="C301" s="6">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D301" s="6">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E301" s="6">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="F301" s="6">
         <v>1</v>
@@ -9478,13 +9802,13 @@
         <v>607</v>
       </c>
       <c r="C302" s="6">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D302" s="6">
-        <v>31.3</v>
+        <v>44</v>
       </c>
       <c r="E302" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F302" s="6">
         <v>1</v>
@@ -9498,13 +9822,13 @@
         <v>609</v>
       </c>
       <c r="C303" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D303" s="6">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E303" s="6">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F303" s="6">
         <v>1</v>
@@ -9518,13 +9842,13 @@
         <v>611</v>
       </c>
       <c r="C304" s="6">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D304" s="6">
-        <v>5.5</v>
+        <v>44</v>
       </c>
       <c r="E304" s="6">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="F304" s="6">
         <v>1</v>
@@ -9538,13 +9862,13 @@
         <v>613</v>
       </c>
       <c r="C305" s="6">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D305" s="6">
-        <v>21.3</v>
+        <v>44</v>
       </c>
       <c r="E305" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F305" s="6">
         <v>1</v>
@@ -9558,13 +9882,13 @@
         <v>615</v>
       </c>
       <c r="C306" s="6">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D306" s="6">
-        <v>35.3</v>
+        <v>40</v>
       </c>
       <c r="E306" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F306" s="6">
         <v>1</v>
@@ -9578,13 +9902,13 @@
         <v>617</v>
       </c>
       <c r="C307" s="6">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D307" s="6">
-        <v>17</v>
+        <v>31.4</v>
       </c>
       <c r="E307" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F307" s="6">
         <v>1</v>
@@ -9598,13 +9922,13 @@
         <v>619</v>
       </c>
       <c r="C308" s="6">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D308" s="6">
-        <v>20</v>
+        <v>31.3</v>
       </c>
       <c r="E308" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F308" s="6">
         <v>1</v>
@@ -9618,13 +9942,13 @@
         <v>621</v>
       </c>
       <c r="C309" s="6">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D309" s="6">
-        <v>25.1</v>
+        <v>31.3</v>
       </c>
       <c r="E309" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F309" s="6">
         <v>1</v>
@@ -9638,13 +9962,13 @@
         <v>623</v>
       </c>
       <c r="C310" s="6">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D310" s="6">
-        <v>48.4</v>
+        <v>31.3</v>
       </c>
       <c r="E310" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F310" s="6">
         <v>1</v>
@@ -9658,13 +9982,13 @@
         <v>625</v>
       </c>
       <c r="C311" s="6">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D311" s="6">
-        <v>38</v>
+        <v>31.3</v>
       </c>
       <c r="E311" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F311" s="6">
         <v>1</v>
@@ -9678,13 +10002,13 @@
         <v>627</v>
       </c>
       <c r="C312" s="6">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D312" s="6">
-        <v>30</v>
+        <v>31.3</v>
       </c>
       <c r="E312" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F312" s="6">
         <v>1</v>
@@ -9698,13 +10022,13 @@
         <v>629</v>
       </c>
       <c r="C313" s="6">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D313" s="6">
-        <v>6</v>
+        <v>31.3</v>
       </c>
       <c r="E313" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F313" s="6">
         <v>1</v>
@@ -9718,13 +10042,13 @@
         <v>631</v>
       </c>
       <c r="C314" s="6">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D314" s="6">
-        <v>60</v>
+        <v>31.3</v>
       </c>
       <c r="E314" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F314" s="6">
         <v>1</v>
@@ -9738,13 +10062,13 @@
         <v>633</v>
       </c>
       <c r="C315" s="6">
-        <v>220</v>
+        <v>6</v>
       </c>
       <c r="D315" s="6">
-        <v>124.5</v>
+        <v>31.3</v>
       </c>
       <c r="E315" s="6">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F315" s="6">
         <v>1</v>
@@ -9758,13 +10082,13 @@
         <v>635</v>
       </c>
       <c r="C316" s="6">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="D316" s="6">
-        <v>25</v>
+        <v>31.3</v>
       </c>
       <c r="E316" s="6">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F316" s="6">
         <v>1</v>
@@ -9778,13 +10102,13 @@
         <v>637</v>
       </c>
       <c r="C317" s="6">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D317" s="6">
-        <v>77</v>
+        <v>31.3</v>
       </c>
       <c r="E317" s="6">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F317" s="6">
         <v>1</v>
@@ -9798,13 +10122,13 @@
         <v>639</v>
       </c>
       <c r="C318" s="6">
-        <v>203</v>
+        <v>2</v>
       </c>
       <c r="D318" s="6">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="E318" s="6">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F318" s="6">
         <v>1</v>
@@ -9818,13 +10142,13 @@
         <v>641</v>
       </c>
       <c r="C319" s="6">
-        <v>181</v>
+        <v>94</v>
       </c>
       <c r="D319" s="6">
-        <v>75.59999999999999</v>
+        <v>428.3</v>
       </c>
       <c r="E319" s="6">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F319" s="6">
         <v>1</v>
@@ -9838,13 +10162,13 @@
         <v>643</v>
       </c>
       <c r="C320" s="6">
-        <v>220</v>
+        <v>56</v>
       </c>
       <c r="D320" s="6">
-        <v>59.4</v>
+        <v>222.6</v>
       </c>
       <c r="E320" s="6">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F320" s="6">
         <v>1</v>
@@ -9858,13 +10182,13 @@
         <v>645</v>
       </c>
       <c r="C321" s="6">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="D321" s="6">
-        <v>52</v>
+        <v>71.5</v>
       </c>
       <c r="E321" s="6">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F321" s="6">
         <v>1</v>
@@ -9878,13 +10202,13 @@
         <v>647</v>
       </c>
       <c r="C322" s="6">
-        <v>138</v>
+        <v>22</v>
       </c>
       <c r="D322" s="6">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="E322" s="6">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F322" s="6">
         <v>1</v>
@@ -9898,13 +10222,13 @@
         <v>649</v>
       </c>
       <c r="C323" s="6">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D323" s="6">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E323" s="6">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F323" s="6">
         <v>1</v>
@@ -9918,13 +10242,13 @@
         <v>651</v>
       </c>
       <c r="C324" s="6">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="D324" s="6">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E324" s="6">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F324" s="6">
         <v>1</v>
@@ -9938,13 +10262,13 @@
         <v>653</v>
       </c>
       <c r="C325" s="6">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="D325" s="6">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="E325" s="6">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F325" s="6">
         <v>1</v>
@@ -9958,13 +10282,13 @@
         <v>655</v>
       </c>
       <c r="C326" s="6">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="D326" s="6">
-        <v>50.4</v>
+        <v>31.3</v>
       </c>
       <c r="E326" s="6">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F326" s="6">
         <v>1</v>
@@ -9978,13 +10302,13 @@
         <v>657</v>
       </c>
       <c r="C327" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D327" s="6">
-        <v>3.8</v>
+        <v>6</v>
       </c>
       <c r="E327" s="6">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F327" s="6">
         <v>1</v>
@@ -9998,13 +10322,13 @@
         <v>659</v>
       </c>
       <c r="C328" s="6">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D328" s="6">
-        <v>0.7</v>
+        <v>5.5</v>
       </c>
       <c r="E328" s="6">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F328" s="6">
         <v>1</v>
@@ -10018,13 +10342,13 @@
         <v>661</v>
       </c>
       <c r="C329" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D329" s="6">
-        <v>4.7</v>
+        <v>21.3</v>
       </c>
       <c r="E329" s="6">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F329" s="6">
         <v>1</v>
@@ -10038,13 +10362,13 @@
         <v>663</v>
       </c>
       <c r="C330" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D330" s="6">
-        <v>5.4</v>
+        <v>35.3</v>
       </c>
       <c r="E330" s="6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F330" s="6">
         <v>1</v>
@@ -10058,13 +10382,13 @@
         <v>665</v>
       </c>
       <c r="C331" s="6">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D331" s="6">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E331" s="6">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F331" s="6">
         <v>1</v>
@@ -10078,13 +10402,13 @@
         <v>667</v>
       </c>
       <c r="C332" s="6">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D332" s="6">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E332" s="6">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F332" s="6">
         <v>1</v>
@@ -10098,10 +10422,10 @@
         <v>669</v>
       </c>
       <c r="C333" s="6">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D333" s="6">
-        <v>11</v>
+        <v>25.1</v>
       </c>
       <c r="E333" s="6">
         <v>16</v>
@@ -10118,13 +10442,13 @@
         <v>671</v>
       </c>
       <c r="C334" s="6">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D334" s="6">
-        <v>13</v>
+        <v>48.4</v>
       </c>
       <c r="E334" s="6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F334" s="6">
         <v>1</v>
@@ -10138,13 +10462,13 @@
         <v>673</v>
       </c>
       <c r="C335" s="6">
+        <v>36</v>
+      </c>
+      <c r="D335" s="6">
+        <v>38</v>
+      </c>
+      <c r="E335" s="6">
         <v>16</v>
-      </c>
-      <c r="D335" s="6">
-        <v>8</v>
-      </c>
-      <c r="E335" s="6">
-        <v>25</v>
       </c>
       <c r="F335" s="6">
         <v>1</v>
@@ -10158,13 +10482,13 @@
         <v>675</v>
       </c>
       <c r="C336" s="6">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D336" s="6">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E336" s="6">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F336" s="6">
         <v>1</v>
@@ -10178,13 +10502,13 @@
         <v>677</v>
       </c>
       <c r="C337" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D337" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E337" s="6">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F337" s="6">
         <v>1</v>
@@ -10198,13 +10522,13 @@
         <v>679</v>
       </c>
       <c r="C338" s="6">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D338" s="6">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="E338" s="6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F338" s="6">
         <v>1</v>
@@ -10218,13 +10542,13 @@
         <v>681</v>
       </c>
       <c r="C339" s="6">
-        <v>22</v>
+        <v>220</v>
       </c>
       <c r="D339" s="6">
-        <v>65</v>
+        <v>124.5</v>
       </c>
       <c r="E339" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F339" s="6">
         <v>1</v>
@@ -10238,13 +10562,13 @@
         <v>683</v>
       </c>
       <c r="C340" s="6">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="D340" s="6">
-        <v>0.6</v>
+        <v>25</v>
       </c>
       <c r="E340" s="6">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F340" s="6">
         <v>1</v>
@@ -10258,13 +10582,13 @@
         <v>685</v>
       </c>
       <c r="C341" s="6">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D341" s="6">
-        <v>15.8</v>
+        <v>77</v>
       </c>
       <c r="E341" s="6">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F341" s="6">
         <v>1</v>
@@ -10278,13 +10602,13 @@
         <v>687</v>
       </c>
       <c r="C342" s="6">
-        <v>14</v>
+        <v>203</v>
       </c>
       <c r="D342" s="6">
-        <v>14.3</v>
+        <v>76</v>
       </c>
       <c r="E342" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F342" s="6">
         <v>1</v>
@@ -10298,13 +10622,13 @@
         <v>689</v>
       </c>
       <c r="C343" s="6">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="D343" s="6">
-        <v>410</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="E343" s="6">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F343" s="6">
         <v>1</v>
@@ -10318,13 +10642,13 @@
         <v>691</v>
       </c>
       <c r="C344" s="6">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="D344" s="6">
-        <v>11</v>
+        <v>59.4</v>
       </c>
       <c r="E344" s="6">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F344" s="6">
         <v>1</v>
@@ -10338,13 +10662,13 @@
         <v>693</v>
       </c>
       <c r="C345" s="6">
-        <v>3</v>
+        <v>188</v>
       </c>
       <c r="D345" s="6">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E345" s="6">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F345" s="6">
         <v>1</v>
@@ -10358,13 +10682,13 @@
         <v>695</v>
       </c>
       <c r="C346" s="6">
-        <v>5</v>
+        <v>138</v>
       </c>
       <c r="D346" s="6">
-        <v>15.5</v>
+        <v>52</v>
       </c>
       <c r="E346" s="6">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F346" s="6">
         <v>1</v>
@@ -10378,13 +10702,13 @@
         <v>697</v>
       </c>
       <c r="C347" s="6">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D347" s="6">
-        <v>33.2</v>
+        <v>22</v>
       </c>
       <c r="E347" s="6">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F347" s="6">
         <v>1</v>
@@ -10398,13 +10722,13 @@
         <v>699</v>
       </c>
       <c r="C348" s="6">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="D348" s="6">
-        <v>26.2</v>
+        <v>51</v>
       </c>
       <c r="E348" s="6">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F348" s="6">
         <v>1</v>
@@ -10418,13 +10742,13 @@
         <v>701</v>
       </c>
       <c r="C349" s="6">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="D349" s="6">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="E349" s="6">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F349" s="6">
         <v>1</v>
@@ -10438,13 +10762,13 @@
         <v>703</v>
       </c>
       <c r="C350" s="6">
-        <v>167.31</v>
+        <v>66</v>
       </c>
       <c r="D350" s="6">
-        <v>485</v>
+        <v>50.4</v>
       </c>
       <c r="E350" s="6">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F350" s="6">
         <v>1</v>
@@ -10458,13 +10782,13 @@
         <v>705</v>
       </c>
       <c r="C351" s="6">
-        <v>43.47</v>
+        <v>1</v>
       </c>
       <c r="D351" s="6">
-        <v>118.61</v>
+        <v>3.8</v>
       </c>
       <c r="E351" s="6">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F351" s="6">
         <v>1</v>
@@ -10478,13 +10802,13 @@
         <v>707</v>
       </c>
       <c r="C352" s="6">
-        <v>99.67</v>
+        <v>1</v>
       </c>
       <c r="D352" s="6">
-        <v>118.61</v>
+        <v>0.7</v>
       </c>
       <c r="E352" s="6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F352" s="6">
         <v>1</v>
@@ -10498,13 +10822,13 @@
         <v>709</v>
       </c>
       <c r="C353" s="6">
-        <v>34.58</v>
+        <v>1</v>
       </c>
       <c r="D353" s="6">
-        <v>104.31</v>
+        <v>4.7</v>
       </c>
       <c r="E353" s="6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F353" s="6">
         <v>1</v>
@@ -10518,13 +10842,13 @@
         <v>711</v>
       </c>
       <c r="C354" s="6">
-        <v>45.49</v>
+        <v>1</v>
       </c>
       <c r="D354" s="6">
-        <v>110</v>
+        <v>5.4</v>
       </c>
       <c r="E354" s="6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F354" s="6">
         <v>1</v>
@@ -10538,13 +10862,13 @@
         <v>713</v>
       </c>
       <c r="C355" s="6">
-        <v>194.66</v>
+        <v>7</v>
       </c>
       <c r="D355" s="6">
-        <v>561.2</v>
+        <v>27</v>
       </c>
       <c r="E355" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F355" s="6">
         <v>1</v>
@@ -10558,10 +10882,10 @@
         <v>715</v>
       </c>
       <c r="C356" s="6">
-        <v>321.56</v>
+        <v>1</v>
       </c>
       <c r="D356" s="6">
-        <v>850.95</v>
+        <v>2</v>
       </c>
       <c r="E356" s="6">
         <v>12</v>
@@ -10578,13 +10902,13 @@
         <v>717</v>
       </c>
       <c r="C357" s="6">
-        <v>28.94</v>
+        <v>11</v>
       </c>
       <c r="D357" s="6">
-        <v>24.88</v>
+        <v>11</v>
       </c>
       <c r="E357" s="6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F357" s="6">
         <v>1</v>
@@ -10598,13 +10922,13 @@
         <v>719</v>
       </c>
       <c r="C358" s="6">
-        <v>43.34</v>
+        <v>18</v>
       </c>
       <c r="D358" s="6">
-        <v>24.18</v>
+        <v>13</v>
       </c>
       <c r="E358" s="6">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F358" s="6">
         <v>1</v>
@@ -10618,13 +10942,13 @@
         <v>721</v>
       </c>
       <c r="C359" s="6">
-        <v>19.21</v>
+        <v>16</v>
       </c>
       <c r="D359" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E359" s="6">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F359" s="6">
         <v>1</v>
@@ -10638,13 +10962,13 @@
         <v>723</v>
       </c>
       <c r="C360" s="6">
-        <v>195.6</v>
+        <v>8</v>
       </c>
       <c r="D360" s="6">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E360" s="6">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F360" s="6">
         <v>1</v>
@@ -10658,13 +10982,13 @@
         <v>725</v>
       </c>
       <c r="C361" s="6">
-        <v>31.58</v>
+        <v>1</v>
       </c>
       <c r="D361" s="6">
-        <v>145.52</v>
+        <v>4</v>
       </c>
       <c r="E361" s="6">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F361" s="6">
         <v>1</v>
@@ -10678,13 +11002,13 @@
         <v>727</v>
       </c>
       <c r="C362" s="6">
-        <v>34.53</v>
+        <v>1</v>
       </c>
       <c r="D362" s="6">
-        <v>12.17</v>
+        <v>3</v>
       </c>
       <c r="E362" s="6">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F362" s="6">
         <v>1</v>
@@ -10698,15 +11022,1073 @@
         <v>729</v>
       </c>
       <c r="C363" s="6">
+        <v>22</v>
+      </c>
+      <c r="D363" s="6">
+        <v>65</v>
+      </c>
+      <c r="E363" s="6">
+        <v>10</v>
+      </c>
+      <c r="F363" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" ht="13.55" customHeight="1">
+      <c r="A364" t="s" s="5">
+        <v>730</v>
+      </c>
+      <c r="B364" t="s" s="5">
+        <v>731</v>
+      </c>
+      <c r="C364" s="6">
+        <v>2</v>
+      </c>
+      <c r="D364" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="E364" s="6">
+        <v>25</v>
+      </c>
+      <c r="F364" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" ht="13.55" customHeight="1">
+      <c r="A365" t="s" s="5">
+        <v>732</v>
+      </c>
+      <c r="B365" t="s" s="5">
+        <v>733</v>
+      </c>
+      <c r="C365" s="6">
+        <v>3</v>
+      </c>
+      <c r="D365" s="6">
+        <v>15.8</v>
+      </c>
+      <c r="E365" s="6">
+        <v>10</v>
+      </c>
+      <c r="F365" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" ht="13.55" customHeight="1">
+      <c r="A366" t="s" s="5">
+        <v>734</v>
+      </c>
+      <c r="B366" t="s" s="5">
+        <v>735</v>
+      </c>
+      <c r="C366" s="6">
+        <v>14</v>
+      </c>
+      <c r="D366" s="6">
+        <v>14.3</v>
+      </c>
+      <c r="E366" s="6">
+        <v>16</v>
+      </c>
+      <c r="F366" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" ht="13.55" customHeight="1">
+      <c r="A367" t="s" s="5">
+        <v>736</v>
+      </c>
+      <c r="B367" t="s" s="5">
+        <v>737</v>
+      </c>
+      <c r="C367" s="6">
+        <v>153</v>
+      </c>
+      <c r="D367" s="6">
+        <v>410</v>
+      </c>
+      <c r="E367" s="6">
+        <v>12</v>
+      </c>
+      <c r="F367" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" ht="13.55" customHeight="1">
+      <c r="A368" t="s" s="5">
+        <v>738</v>
+      </c>
+      <c r="B368" t="s" s="5">
+        <v>739</v>
+      </c>
+      <c r="C368" s="6">
+        <v>4</v>
+      </c>
+      <c r="D368" s="6">
+        <v>11</v>
+      </c>
+      <c r="E368" s="6">
+        <v>12</v>
+      </c>
+      <c r="F368" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" ht="13.55" customHeight="1">
+      <c r="A369" t="s" s="5">
+        <v>740</v>
+      </c>
+      <c r="B369" t="s" s="5">
+        <v>741</v>
+      </c>
+      <c r="C369" s="6">
+        <v>3</v>
+      </c>
+      <c r="D369" s="6">
+        <v>10</v>
+      </c>
+      <c r="E369" s="6">
+        <v>6</v>
+      </c>
+      <c r="F369" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" ht="13.55" customHeight="1">
+      <c r="A370" t="s" s="5">
+        <v>742</v>
+      </c>
+      <c r="B370" t="s" s="5">
+        <v>743</v>
+      </c>
+      <c r="C370" s="6">
+        <v>5</v>
+      </c>
+      <c r="D370" s="6">
+        <v>15.5</v>
+      </c>
+      <c r="E370" s="6">
+        <v>10</v>
+      </c>
+      <c r="F370" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" ht="13.55" customHeight="1">
+      <c r="A371" t="s" s="5">
+        <v>744</v>
+      </c>
+      <c r="B371" t="s" s="5">
+        <v>745</v>
+      </c>
+      <c r="C371" s="6">
+        <v>39</v>
+      </c>
+      <c r="D371" s="6">
+        <v>33.2</v>
+      </c>
+      <c r="E371" s="6">
+        <v>16</v>
+      </c>
+      <c r="F371" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" ht="13.55" customHeight="1">
+      <c r="A372" t="s" s="5">
+        <v>746</v>
+      </c>
+      <c r="B372" t="s" s="5">
+        <v>747</v>
+      </c>
+      <c r="C372" s="6">
+        <v>4</v>
+      </c>
+      <c r="D372" s="6">
+        <v>26.2</v>
+      </c>
+      <c r="E372" s="6">
+        <v>6</v>
+      </c>
+      <c r="F372" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" ht="13.55" customHeight="1">
+      <c r="A373" t="s" s="5">
+        <v>748</v>
+      </c>
+      <c r="B373" t="s" s="5">
+        <v>749</v>
+      </c>
+      <c r="C373" s="6">
+        <v>37</v>
+      </c>
+      <c r="D373" s="6">
+        <v>155</v>
+      </c>
+      <c r="E373" s="6">
+        <v>10</v>
+      </c>
+      <c r="F373" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" ht="13.55" customHeight="1">
+      <c r="A374" t="s" s="5">
+        <v>750</v>
+      </c>
+      <c r="B374" t="s" s="5">
+        <v>751</v>
+      </c>
+      <c r="C374" s="6">
+        <v>9</v>
+      </c>
+      <c r="D374" s="6">
+        <v>115</v>
+      </c>
+      <c r="E374" s="6">
+        <v>10</v>
+      </c>
+      <c r="F374" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" ht="13.55" customHeight="1">
+      <c r="A375" t="s" s="5">
+        <v>752</v>
+      </c>
+      <c r="B375" t="s" s="5">
+        <v>753</v>
+      </c>
+      <c r="C375" s="6">
+        <v>1</v>
+      </c>
+      <c r="D375" s="6">
+        <v>2</v>
+      </c>
+      <c r="E375" s="6">
+        <v>8</v>
+      </c>
+      <c r="F375" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" ht="13.55" customHeight="1">
+      <c r="A376" t="s" s="5">
+        <v>754</v>
+      </c>
+      <c r="B376" t="s" s="5">
+        <v>755</v>
+      </c>
+      <c r="C376" s="6">
+        <v>1</v>
+      </c>
+      <c r="D376" s="6">
+        <v>1</v>
+      </c>
+      <c r="E376" s="6">
+        <v>14</v>
+      </c>
+      <c r="F376" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" ht="13.55" customHeight="1">
+      <c r="A377" t="s" s="5">
+        <v>756</v>
+      </c>
+      <c r="B377" t="s" s="5">
+        <v>757</v>
+      </c>
+      <c r="C377" s="6">
+        <v>5</v>
+      </c>
+      <c r="D377" s="6">
+        <v>4</v>
+      </c>
+      <c r="E377" s="6">
+        <v>16</v>
+      </c>
+      <c r="F377" s="7"/>
+    </row>
+    <row r="378" ht="13.55" customHeight="1">
+      <c r="A378" t="s" s="5">
+        <v>758</v>
+      </c>
+      <c r="B378" t="s" s="5">
+        <v>759</v>
+      </c>
+      <c r="C378" s="6">
+        <v>404</v>
+      </c>
+      <c r="D378" s="6">
+        <v>214.3</v>
+      </c>
+      <c r="E378" s="6">
+        <v>25</v>
+      </c>
+      <c r="F378" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" ht="13.55" customHeight="1">
+      <c r="A379" t="s" s="5">
+        <v>760</v>
+      </c>
+      <c r="B379" t="s" s="5">
+        <v>761</v>
+      </c>
+      <c r="C379" s="6">
+        <v>202</v>
+      </c>
+      <c r="D379" s="6">
+        <v>108</v>
+      </c>
+      <c r="E379" s="6">
+        <v>25</v>
+      </c>
+      <c r="F379" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" ht="13.55" customHeight="1">
+      <c r="A380" t="s" s="5">
+        <v>762</v>
+      </c>
+      <c r="B380" t="s" s="5">
+        <v>763</v>
+      </c>
+      <c r="C380" s="6">
+        <v>82</v>
+      </c>
+      <c r="D380" s="6">
+        <v>32.6</v>
+      </c>
+      <c r="E380" s="6">
+        <v>25</v>
+      </c>
+      <c r="F380" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" ht="13.55" customHeight="1">
+      <c r="A381" t="s" s="5">
+        <v>764</v>
+      </c>
+      <c r="B381" t="s" s="5">
+        <v>765</v>
+      </c>
+      <c r="C381" s="6">
+        <v>27</v>
+      </c>
+      <c r="D381" s="6">
+        <v>20</v>
+      </c>
+      <c r="E381" s="6">
+        <v>25</v>
+      </c>
+      <c r="F381" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" ht="13.55" customHeight="1">
+      <c r="A382" t="s" s="5">
+        <v>766</v>
+      </c>
+      <c r="B382" t="s" s="5">
+        <v>767</v>
+      </c>
+      <c r="C382" s="6">
+        <v>890</v>
+      </c>
+      <c r="D382" s="6">
+        <v>545</v>
+      </c>
+      <c r="E382" s="6">
+        <v>25</v>
+      </c>
+      <c r="F382" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" ht="13.55" customHeight="1">
+      <c r="A383" t="s" s="5">
+        <v>768</v>
+      </c>
+      <c r="B383" t="s" s="5">
+        <v>769</v>
+      </c>
+      <c r="C383" s="6">
+        <v>7</v>
+      </c>
+      <c r="D383" s="6">
+        <v>42.3</v>
+      </c>
+      <c r="E383" s="6">
+        <v>6</v>
+      </c>
+      <c r="F383" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" ht="13.55" customHeight="1">
+      <c r="A384" t="s" s="5">
+        <v>770</v>
+      </c>
+      <c r="B384" t="s" s="5">
+        <v>771</v>
+      </c>
+      <c r="C384" s="6">
+        <v>2</v>
+      </c>
+      <c r="D384" s="6">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="E384" s="6">
+        <v>8</v>
+      </c>
+      <c r="F384" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" ht="13.55" customHeight="1">
+      <c r="A385" t="s" s="5">
+        <v>772</v>
+      </c>
+      <c r="B385" t="s" s="5">
+        <v>773</v>
+      </c>
+      <c r="C385" s="6">
+        <v>1</v>
+      </c>
+      <c r="D385" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="E385" s="6">
+        <v>10</v>
+      </c>
+      <c r="F385" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" ht="13.55" customHeight="1">
+      <c r="A386" t="s" s="5">
+        <v>774</v>
+      </c>
+      <c r="B386" t="s" s="5">
+        <v>775</v>
+      </c>
+      <c r="C386" s="6">
+        <v>1</v>
+      </c>
+      <c r="D386" s="6">
+        <v>2.3</v>
+      </c>
+      <c r="E386" s="6">
+        <v>12</v>
+      </c>
+      <c r="F386" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" ht="13.55" customHeight="1">
+      <c r="A387" t="s" s="5">
+        <v>776</v>
+      </c>
+      <c r="B387" t="s" s="5">
+        <v>777</v>
+      </c>
+      <c r="C387" s="6">
+        <v>74</v>
+      </c>
+      <c r="D387" s="6">
+        <v>604</v>
+      </c>
+      <c r="E387" s="6">
+        <v>12</v>
+      </c>
+      <c r="F387" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" ht="13.55" customHeight="1">
+      <c r="A388" t="s" s="5">
+        <v>778</v>
+      </c>
+      <c r="B388" t="s" s="5">
+        <v>779</v>
+      </c>
+      <c r="C388" s="6">
+        <v>156</v>
+      </c>
+      <c r="D388" s="6">
+        <v>371</v>
+      </c>
+      <c r="E388" s="6">
+        <v>12</v>
+      </c>
+      <c r="F388" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" ht="13.55" customHeight="1">
+      <c r="A389" t="s" s="5">
+        <v>780</v>
+      </c>
+      <c r="B389" t="s" s="5">
+        <v>781</v>
+      </c>
+      <c r="C389" s="6">
+        <v>15</v>
+      </c>
+      <c r="D389" s="6">
+        <v>59</v>
+      </c>
+      <c r="E389" s="6">
+        <v>6</v>
+      </c>
+      <c r="F389" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" ht="13.55" customHeight="1">
+      <c r="A390" t="s" s="5">
+        <v>782</v>
+      </c>
+      <c r="B390" t="s" s="5">
+        <v>783</v>
+      </c>
+      <c r="C390" s="6">
+        <v>18</v>
+      </c>
+      <c r="D390" s="6">
+        <v>64</v>
+      </c>
+      <c r="E390" s="6">
+        <v>8</v>
+      </c>
+      <c r="F390" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" ht="13.55" customHeight="1">
+      <c r="A391" t="s" s="5">
+        <v>784</v>
+      </c>
+      <c r="B391" t="s" s="5">
+        <v>785</v>
+      </c>
+      <c r="C391" s="6">
+        <v>8</v>
+      </c>
+      <c r="D391" s="6">
+        <v>32</v>
+      </c>
+      <c r="E391" s="6">
+        <v>10</v>
+      </c>
+      <c r="F391" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" ht="13.55" customHeight="1">
+      <c r="A392" t="s" s="5">
+        <v>786</v>
+      </c>
+      <c r="B392" t="s" s="5">
+        <v>787</v>
+      </c>
+      <c r="C392" s="6">
+        <v>2</v>
+      </c>
+      <c r="D392" s="6">
+        <v>4</v>
+      </c>
+      <c r="E392" s="6">
+        <v>12</v>
+      </c>
+      <c r="F392" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" ht="13.55" customHeight="1">
+      <c r="A393" t="s" s="5">
+        <v>788</v>
+      </c>
+      <c r="B393" t="s" s="5">
+        <v>789</v>
+      </c>
+      <c r="C393" s="6">
+        <v>10</v>
+      </c>
+      <c r="D393" s="6">
+        <v>6</v>
+      </c>
+      <c r="E393" s="6">
+        <v>20</v>
+      </c>
+      <c r="F393" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" ht="13.55" customHeight="1">
+      <c r="A394" t="s" s="5">
+        <v>790</v>
+      </c>
+      <c r="B394" t="s" s="5">
+        <v>791</v>
+      </c>
+      <c r="C394" s="6">
+        <v>14</v>
+      </c>
+      <c r="D394" s="6">
+        <v>5</v>
+      </c>
+      <c r="E394" s="6">
+        <v>32</v>
+      </c>
+      <c r="F394" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" ht="13.55" customHeight="1">
+      <c r="A395" t="s" s="5">
+        <v>792</v>
+      </c>
+      <c r="B395" t="s" s="5">
+        <v>793</v>
+      </c>
+      <c r="C395" s="6">
+        <v>120</v>
+      </c>
+      <c r="D395" s="6">
+        <v>345</v>
+      </c>
+      <c r="E395" s="6">
+        <v>12</v>
+      </c>
+      <c r="F395" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" ht="13.55" customHeight="1">
+      <c r="A396" t="s" s="5">
+        <v>794</v>
+      </c>
+      <c r="B396" t="s" s="5">
+        <v>795</v>
+      </c>
+      <c r="C396" s="6">
+        <v>34</v>
+      </c>
+      <c r="D396" s="6">
+        <v>98</v>
+      </c>
+      <c r="E396" s="6">
+        <v>12</v>
+      </c>
+      <c r="F396" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" ht="13.55" customHeight="1">
+      <c r="A397" t="s" s="5">
+        <v>796</v>
+      </c>
+      <c r="B397" t="s" s="5">
+        <v>797</v>
+      </c>
+      <c r="C397" s="6">
+        <v>2</v>
+      </c>
+      <c r="D397" s="6">
+        <v>8</v>
+      </c>
+      <c r="E397" s="6">
+        <v>6</v>
+      </c>
+      <c r="F397" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" ht="13.55" customHeight="1">
+      <c r="A398" t="s" s="5">
+        <v>798</v>
+      </c>
+      <c r="B398" t="s" s="5">
+        <v>799</v>
+      </c>
+      <c r="C398" s="6">
+        <v>12</v>
+      </c>
+      <c r="D398" s="6">
+        <v>74</v>
+      </c>
+      <c r="E398" s="6">
+        <v>8</v>
+      </c>
+      <c r="F398" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" ht="13.55" customHeight="1">
+      <c r="A399" t="s" s="5">
+        <v>800</v>
+      </c>
+      <c r="B399" t="s" s="5">
+        <v>801</v>
+      </c>
+      <c r="C399" s="6">
+        <v>3</v>
+      </c>
+      <c r="D399" s="6">
+        <v>12</v>
+      </c>
+      <c r="E399" s="6">
+        <v>12</v>
+      </c>
+      <c r="F399" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" ht="13.55" customHeight="1">
+      <c r="A400" t="s" s="5">
+        <v>802</v>
+      </c>
+      <c r="B400" t="s" s="5">
+        <v>803</v>
+      </c>
+      <c r="C400" s="6">
+        <v>20</v>
+      </c>
+      <c r="D400" s="6">
+        <v>20</v>
+      </c>
+      <c r="E400" s="6">
+        <v>12</v>
+      </c>
+      <c r="F400" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" ht="13.55" customHeight="1">
+      <c r="A401" t="s" s="5">
+        <v>804</v>
+      </c>
+      <c r="B401" t="s" s="5">
+        <v>805</v>
+      </c>
+      <c r="C401" s="6">
+        <v>1</v>
+      </c>
+      <c r="D401" s="6">
+        <v>4</v>
+      </c>
+      <c r="E401" s="6">
+        <v>8</v>
+      </c>
+      <c r="F401" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" ht="13.55" customHeight="1">
+      <c r="A402" t="s" s="5">
+        <v>806</v>
+      </c>
+      <c r="B402" t="s" s="5">
+        <v>807</v>
+      </c>
+      <c r="C402" s="6">
+        <v>29</v>
+      </c>
+      <c r="D402" s="6">
+        <v>1</v>
+      </c>
+      <c r="E402" s="6">
+        <v>14</v>
+      </c>
+      <c r="F402" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" ht="13.55" customHeight="1">
+      <c r="A403" t="s" s="5">
+        <v>808</v>
+      </c>
+      <c r="B403" t="s" s="5">
+        <v>809</v>
+      </c>
+      <c r="C403" s="6">
+        <v>167.31</v>
+      </c>
+      <c r="D403" s="6">
+        <v>485</v>
+      </c>
+      <c r="E403" s="6">
+        <v>12</v>
+      </c>
+      <c r="F403" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" ht="13.55" customHeight="1">
+      <c r="A404" t="s" s="5">
+        <v>810</v>
+      </c>
+      <c r="B404" t="s" s="5">
+        <v>811</v>
+      </c>
+      <c r="C404" s="6">
+        <v>43.47</v>
+      </c>
+      <c r="D404" s="6">
+        <v>118.61</v>
+      </c>
+      <c r="E404" s="6">
+        <v>12</v>
+      </c>
+      <c r="F404" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" ht="13.55" customHeight="1">
+      <c r="A405" t="s" s="5">
+        <v>812</v>
+      </c>
+      <c r="B405" t="s" s="5">
+        <v>813</v>
+      </c>
+      <c r="C405" s="6">
+        <v>99.67</v>
+      </c>
+      <c r="D405" s="6">
+        <v>118.61</v>
+      </c>
+      <c r="E405" s="6">
+        <v>12</v>
+      </c>
+      <c r="F405" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" ht="13.55" customHeight="1">
+      <c r="A406" t="s" s="5">
+        <v>814</v>
+      </c>
+      <c r="B406" t="s" s="5">
+        <v>815</v>
+      </c>
+      <c r="C406" s="6">
+        <v>34.58</v>
+      </c>
+      <c r="D406" s="6">
+        <v>104.31</v>
+      </c>
+      <c r="E406" s="6">
+        <v>12</v>
+      </c>
+      <c r="F406" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" ht="13.55" customHeight="1">
+      <c r="A407" t="s" s="5">
+        <v>816</v>
+      </c>
+      <c r="B407" t="s" s="5">
+        <v>817</v>
+      </c>
+      <c r="C407" s="6">
+        <v>45.49</v>
+      </c>
+      <c r="D407" s="6">
+        <v>110</v>
+      </c>
+      <c r="E407" s="6">
+        <v>12</v>
+      </c>
+      <c r="F407" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" ht="13.55" customHeight="1">
+      <c r="A408" t="s" s="5">
+        <v>818</v>
+      </c>
+      <c r="B408" t="s" s="5">
+        <v>819</v>
+      </c>
+      <c r="C408" s="6">
+        <v>194.66</v>
+      </c>
+      <c r="D408" s="6">
+        <v>561.2</v>
+      </c>
+      <c r="E408" s="6">
+        <v>12</v>
+      </c>
+      <c r="F408" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" ht="13.55" customHeight="1">
+      <c r="A409" t="s" s="5">
+        <v>820</v>
+      </c>
+      <c r="B409" t="s" s="5">
+        <v>821</v>
+      </c>
+      <c r="C409" s="6">
+        <v>321.56</v>
+      </c>
+      <c r="D409" s="6">
+        <v>850.95</v>
+      </c>
+      <c r="E409" s="6">
+        <v>12</v>
+      </c>
+      <c r="F409" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" ht="13.55" customHeight="1">
+      <c r="A410" t="s" s="5">
+        <v>822</v>
+      </c>
+      <c r="B410" t="s" s="5">
+        <v>823</v>
+      </c>
+      <c r="C410" s="6">
+        <v>28.94</v>
+      </c>
+      <c r="D410" s="6">
+        <v>24.88</v>
+      </c>
+      <c r="E410" s="6">
+        <v>20</v>
+      </c>
+      <c r="F410" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" ht="13.55" customHeight="1">
+      <c r="A411" t="s" s="5">
+        <v>824</v>
+      </c>
+      <c r="B411" t="s" s="5">
+        <v>825</v>
+      </c>
+      <c r="C411" s="6">
+        <v>43.34</v>
+      </c>
+      <c r="D411" s="6">
+        <v>24.18</v>
+      </c>
+      <c r="E411" s="6">
+        <v>25</v>
+      </c>
+      <c r="F411" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" ht="13.55" customHeight="1">
+      <c r="A412" t="s" s="5">
+        <v>826</v>
+      </c>
+      <c r="B412" t="s" s="5">
+        <v>827</v>
+      </c>
+      <c r="C412" s="6">
+        <v>19.21</v>
+      </c>
+      <c r="D412" s="6">
+        <v>5</v>
+      </c>
+      <c r="E412" s="6">
+        <v>32</v>
+      </c>
+      <c r="F412" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" ht="13.55" customHeight="1">
+      <c r="A413" t="s" s="5">
+        <v>828</v>
+      </c>
+      <c r="B413" t="s" s="5">
+        <v>829</v>
+      </c>
+      <c r="C413" s="6">
+        <v>195.6</v>
+      </c>
+      <c r="D413" s="6">
+        <v>17</v>
+      </c>
+      <c r="E413" s="6">
+        <v>32</v>
+      </c>
+      <c r="F413" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" ht="13.55" customHeight="1">
+      <c r="A414" t="s" s="5">
+        <v>830</v>
+      </c>
+      <c r="B414" t="s" s="5">
+        <v>831</v>
+      </c>
+      <c r="C414" s="6">
+        <v>31.58</v>
+      </c>
+      <c r="D414" s="6">
+        <v>145.52</v>
+      </c>
+      <c r="E414" s="6">
+        <v>10</v>
+      </c>
+      <c r="F414" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" ht="13.55" customHeight="1">
+      <c r="A415" t="s" s="5">
+        <v>832</v>
+      </c>
+      <c r="B415" t="s" s="5">
+        <v>833</v>
+      </c>
+      <c r="C415" s="6">
+        <v>34.53</v>
+      </c>
+      <c r="D415" s="6">
+        <v>12.17</v>
+      </c>
+      <c r="E415" s="6">
+        <v>25</v>
+      </c>
+      <c r="F415" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" ht="13.55" customHeight="1">
+      <c r="A416" t="s" s="5">
+        <v>834</v>
+      </c>
+      <c r="B416" t="s" s="5">
+        <v>835</v>
+      </c>
+      <c r="C416" s="6">
         <v>9.35</v>
       </c>
-      <c r="D363" s="6">
+      <c r="D416" s="6">
         <v>30</v>
       </c>
-      <c r="E363" s="6">
+      <c r="E416" s="6">
         <v>12</v>
       </c>
-      <c r="F363" s="6">
+      <c r="F416" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update CSV and Excel data files
Updated `data/saved_df_2024_10.csv` and `data/tiempo_final.xlsx` with the latest data. These changes ensure that the dataset is current and accurate for future analyses.
</commit_message>
<xml_diff>
--- a/data/tiempo_final.xlsx
+++ b/data/tiempo_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="890">
   <si>
     <t>timestamp</t>
   </si>
@@ -2519,6 +2519,168 @@
   </si>
   <si>
     <t>bisel de forma 02.slp</t>
+  </si>
+  <si>
+    <t>2024-10-24 09:07:43</t>
+  </si>
+  <si>
+    <t>L_05631.NC</t>
+  </si>
+  <si>
+    <t>2024-10-24 11:11:40</t>
+  </si>
+  <si>
+    <t>L_05558.NC</t>
+  </si>
+  <si>
+    <t>2024-10-24 11:30:46</t>
+  </si>
+  <si>
+    <t>L_05559.NC</t>
+  </si>
+  <si>
+    <t>2024-10-24 11:53:49</t>
+  </si>
+  <si>
+    <t>L_05555.NC</t>
+  </si>
+  <si>
+    <t>2024-10-24 12:31:41</t>
+  </si>
+  <si>
+    <t>L_05556.NC</t>
+  </si>
+  <si>
+    <t>2024-10-24 13:31:28</t>
+  </si>
+  <si>
+    <t>L_05557.NC</t>
+  </si>
+  <si>
+    <t>2024-10-24 13:39:52</t>
+  </si>
+  <si>
+    <t>L_05640.NC</t>
+  </si>
+  <si>
+    <t>2024-10-24 15:53:33</t>
+  </si>
+  <si>
+    <t>L_05647.NC</t>
+  </si>
+  <si>
+    <t>2024-10-25 07:56:20</t>
+  </si>
+  <si>
+    <t>L_05644.NC</t>
+  </si>
+  <si>
+    <t>2024-10-25 11:27:24</t>
+  </si>
+  <si>
+    <t>L_05613.NC</t>
+  </si>
+  <si>
+    <t>2024-10-25 11:36:59</t>
+  </si>
+  <si>
+    <t>L_05616.NC</t>
+  </si>
+  <si>
+    <t>2024-10-25 12:14:50</t>
+  </si>
+  <si>
+    <t>L_05617.NC</t>
+  </si>
+  <si>
+    <t>2024-10-25 14:42:01</t>
+  </si>
+  <si>
+    <t>L_05611.NC</t>
+  </si>
+  <si>
+    <t>2024-10-25 15:59:50</t>
+  </si>
+  <si>
+    <t>L_05609.NC</t>
+  </si>
+  <si>
+    <t>2024-10-28 09:31:17</t>
+  </si>
+  <si>
+    <t>L_05610.NC</t>
+  </si>
+  <si>
+    <t>2024-10-28 10:40:13</t>
+  </si>
+  <si>
+    <t>L_05612.NC</t>
+  </si>
+  <si>
+    <t>2024-10-28 12:45:48</t>
+  </si>
+  <si>
+    <t>L_05618.NC</t>
+  </si>
+  <si>
+    <t>2024-10-28 12:46:42</t>
+  </si>
+  <si>
+    <t>L_05615.NC</t>
+  </si>
+  <si>
+    <t>2024-10-28 13:54:36</t>
+  </si>
+  <si>
+    <t>L_15435.NC</t>
+  </si>
+  <si>
+    <t>2024-10-28 15:40:04</t>
+  </si>
+  <si>
+    <t>L_15427.NC</t>
+  </si>
+  <si>
+    <t>2024-10-29 11:52:36</t>
+  </si>
+  <si>
+    <t>L_05614.NC</t>
+  </si>
+  <si>
+    <t>2024-10-29 14:28:57</t>
+  </si>
+  <si>
+    <t>020130.NC</t>
+  </si>
+  <si>
+    <t>2024-10-29 14:39:55</t>
+  </si>
+  <si>
+    <t>020134.NC</t>
+  </si>
+  <si>
+    <t>2024-10-29 14:51:54</t>
+  </si>
+  <si>
+    <t>020131.NC</t>
+  </si>
+  <si>
+    <t>2024-10-29 14:54:20</t>
+  </si>
+  <si>
+    <t>020133.NC</t>
+  </si>
+  <si>
+    <t>2024-10-29 15:12:04</t>
+  </si>
+  <si>
+    <t>020132.NC</t>
+  </si>
+  <si>
+    <t>2024-10-30 14:48:38</t>
+  </si>
+  <si>
+    <t>020216.NC</t>
   </si>
 </sst>
 </file>
@@ -2624,7 +2786,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -2644,9 +2806,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -3759,18 +3918,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F416"/>
+  <dimension ref="A1:F443"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.9297" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.2344" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.2109" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5078" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5859" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.9688" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11310,7 +11466,9 @@
       <c r="E377" s="6">
         <v>16</v>
       </c>
-      <c r="F377" s="7"/>
+      <c r="F377" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="378" ht="13.55" customHeight="1">
       <c r="A378" t="s" s="5">
@@ -12089,6 +12247,546 @@
         <v>12</v>
       </c>
       <c r="F416" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" ht="13.55" customHeight="1">
+      <c r="A417" t="s" s="5">
+        <v>836</v>
+      </c>
+      <c r="B417" t="s" s="5">
+        <v>837</v>
+      </c>
+      <c r="C417" s="6">
+        <v>25</v>
+      </c>
+      <c r="D417" s="6">
+        <v>110</v>
+      </c>
+      <c r="E417" s="6">
+        <v>10</v>
+      </c>
+      <c r="F417" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" ht="13.55" customHeight="1">
+      <c r="A418" t="s" s="5">
+        <v>838</v>
+      </c>
+      <c r="B418" t="s" s="5">
+        <v>839</v>
+      </c>
+      <c r="C418" s="6">
+        <v>4</v>
+      </c>
+      <c r="D418" s="6">
+        <v>29</v>
+      </c>
+      <c r="E418" s="6">
+        <v>6</v>
+      </c>
+      <c r="F418" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" ht="13.55" customHeight="1">
+      <c r="A419" t="s" s="5">
+        <v>840</v>
+      </c>
+      <c r="B419" t="s" s="5">
+        <v>841</v>
+      </c>
+      <c r="C419" s="6">
+        <v>2</v>
+      </c>
+      <c r="D419" s="6">
+        <v>6</v>
+      </c>
+      <c r="E419" s="6">
+        <v>10</v>
+      </c>
+      <c r="F419" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" ht="13.55" customHeight="1">
+      <c r="A420" t="s" s="5">
+        <v>842</v>
+      </c>
+      <c r="B420" t="s" s="5">
+        <v>843</v>
+      </c>
+      <c r="C420" s="6">
+        <v>4</v>
+      </c>
+      <c r="D420" s="6">
+        <v>17</v>
+      </c>
+      <c r="E420" s="6">
+        <v>4</v>
+      </c>
+      <c r="F420" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" ht="13.55" customHeight="1">
+      <c r="A421" t="s" s="5">
+        <v>844</v>
+      </c>
+      <c r="B421" t="s" s="5">
+        <v>845</v>
+      </c>
+      <c r="C421" s="6">
+        <v>8</v>
+      </c>
+      <c r="D421" s="6">
+        <v>39</v>
+      </c>
+      <c r="E421" s="6">
+        <v>5</v>
+      </c>
+      <c r="F421" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" ht="13.55" customHeight="1">
+      <c r="A422" t="s" s="5">
+        <v>846</v>
+      </c>
+      <c r="B422" t="s" s="5">
+        <v>847</v>
+      </c>
+      <c r="C422" s="6">
+        <v>2</v>
+      </c>
+      <c r="D422" s="6">
+        <v>13.5</v>
+      </c>
+      <c r="E422" s="6">
+        <v>5</v>
+      </c>
+      <c r="F422" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" ht="13.55" customHeight="1">
+      <c r="A423" t="s" s="5">
+        <v>848</v>
+      </c>
+      <c r="B423" t="s" s="5">
+        <v>849</v>
+      </c>
+      <c r="C423" s="6">
+        <v>9</v>
+      </c>
+      <c r="D423" s="6">
+        <v>24.3</v>
+      </c>
+      <c r="E423" s="6">
+        <v>12</v>
+      </c>
+      <c r="F423" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" ht="13.55" customHeight="1">
+      <c r="A424" t="s" s="5">
+        <v>850</v>
+      </c>
+      <c r="B424" t="s" s="5">
+        <v>851</v>
+      </c>
+      <c r="C424" s="6">
+        <v>21</v>
+      </c>
+      <c r="D424" s="6">
+        <v>16</v>
+      </c>
+      <c r="E424" s="6">
+        <v>20</v>
+      </c>
+      <c r="F424" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" ht="13.55" customHeight="1">
+      <c r="A425" t="s" s="5">
+        <v>852</v>
+      </c>
+      <c r="B425" t="s" s="5">
+        <v>853</v>
+      </c>
+      <c r="C425" s="6">
+        <v>32</v>
+      </c>
+      <c r="D425" s="6">
+        <v>30</v>
+      </c>
+      <c r="E425" s="6">
+        <v>18</v>
+      </c>
+      <c r="F425" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" ht="13.55" customHeight="1">
+      <c r="A426" t="s" s="5">
+        <v>854</v>
+      </c>
+      <c r="B426" t="s" s="5">
+        <v>855</v>
+      </c>
+      <c r="C426" s="6">
+        <v>9</v>
+      </c>
+      <c r="D426" s="6">
+        <v>23</v>
+      </c>
+      <c r="E426" s="6">
+        <v>10</v>
+      </c>
+      <c r="F426" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" ht="13.55" customHeight="1">
+      <c r="A427" t="s" s="5">
+        <v>856</v>
+      </c>
+      <c r="B427" t="s" s="5">
+        <v>857</v>
+      </c>
+      <c r="C427" s="6">
+        <v>19</v>
+      </c>
+      <c r="D427" s="6">
+        <v>18</v>
+      </c>
+      <c r="E427" s="6">
+        <v>16</v>
+      </c>
+      <c r="F427" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" ht="13.55" customHeight="1">
+      <c r="A428" t="s" s="5">
+        <v>858</v>
+      </c>
+      <c r="B428" t="s" s="5">
+        <v>859</v>
+      </c>
+      <c r="C428" s="6">
+        <v>5</v>
+      </c>
+      <c r="D428" s="6">
+        <v>4</v>
+      </c>
+      <c r="E428" s="6">
+        <v>18</v>
+      </c>
+      <c r="F428" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" ht="13.55" customHeight="1">
+      <c r="A429" t="s" s="5">
+        <v>860</v>
+      </c>
+      <c r="B429" t="s" s="5">
+        <v>861</v>
+      </c>
+      <c r="C429" s="6">
+        <v>18</v>
+      </c>
+      <c r="D429" s="6">
+        <v>28</v>
+      </c>
+      <c r="E429" s="6">
+        <v>6</v>
+      </c>
+      <c r="F429" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" ht="13.55" customHeight="1">
+      <c r="A430" t="s" s="5">
+        <v>862</v>
+      </c>
+      <c r="B430" t="s" s="5">
+        <v>863</v>
+      </c>
+      <c r="C430" s="6">
+        <v>12</v>
+      </c>
+      <c r="D430" s="6">
+        <v>62</v>
+      </c>
+      <c r="E430" s="6">
+        <v>6</v>
+      </c>
+      <c r="F430" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" ht="13.55" customHeight="1">
+      <c r="A431" t="s" s="5">
+        <v>864</v>
+      </c>
+      <c r="B431" t="s" s="5">
+        <v>865</v>
+      </c>
+      <c r="C431" s="6">
+        <v>3</v>
+      </c>
+      <c r="D431" s="6">
+        <v>29</v>
+      </c>
+      <c r="E431" s="6">
+        <v>6</v>
+      </c>
+      <c r="F431" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" ht="13.55" customHeight="1">
+      <c r="A432" t="s" s="5">
+        <v>866</v>
+      </c>
+      <c r="B432" t="s" s="5">
+        <v>867</v>
+      </c>
+      <c r="C432" s="6">
+        <v>19</v>
+      </c>
+      <c r="D432" s="6">
+        <v>97</v>
+      </c>
+      <c r="E432" s="6">
+        <v>8</v>
+      </c>
+      <c r="F432" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" ht="13.55" customHeight="1">
+      <c r="A433" t="s" s="5">
+        <v>868</v>
+      </c>
+      <c r="B433" t="s" s="5">
+        <v>869</v>
+      </c>
+      <c r="C433" s="6">
+        <v>16</v>
+      </c>
+      <c r="D433" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="E433" s="6">
+        <v>32</v>
+      </c>
+      <c r="F433" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" ht="13.55" customHeight="1">
+      <c r="A434" t="s" s="5">
+        <v>870</v>
+      </c>
+      <c r="B434" t="s" s="5">
+        <v>871</v>
+      </c>
+      <c r="C434" s="6">
+        <v>1</v>
+      </c>
+      <c r="D434" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E434" s="6">
+        <v>14</v>
+      </c>
+      <c r="F434" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" ht="13.55" customHeight="1">
+      <c r="A435" t="s" s="5">
+        <v>872</v>
+      </c>
+      <c r="B435" t="s" s="5">
+        <v>873</v>
+      </c>
+      <c r="C435" s="6">
+        <v>30</v>
+      </c>
+      <c r="D435" s="6">
+        <v>24</v>
+      </c>
+      <c r="E435" s="6">
+        <v>20</v>
+      </c>
+      <c r="F435" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" ht="13.55" customHeight="1">
+      <c r="A436" t="s" s="5">
+        <v>874</v>
+      </c>
+      <c r="B436" t="s" s="5">
+        <v>875</v>
+      </c>
+      <c r="C436" s="6">
+        <v>9</v>
+      </c>
+      <c r="D436" s="6">
+        <v>68</v>
+      </c>
+      <c r="E436" s="6">
+        <v>3</v>
+      </c>
+      <c r="F436" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" ht="13.55" customHeight="1">
+      <c r="A437" t="s" s="5">
+        <v>876</v>
+      </c>
+      <c r="B437" t="s" s="5">
+        <v>877</v>
+      </c>
+      <c r="C437" s="6">
+        <v>14</v>
+      </c>
+      <c r="D437" s="6">
+        <v>38</v>
+      </c>
+      <c r="E437" s="6">
+        <v>12</v>
+      </c>
+      <c r="F437" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" ht="13.55" customHeight="1">
+      <c r="A438" t="s" s="5">
+        <v>878</v>
+      </c>
+      <c r="B438" t="s" s="5">
+        <v>879</v>
+      </c>
+      <c r="C438" s="6">
+        <v>3</v>
+      </c>
+      <c r="D438" s="6">
+        <v>11</v>
+      </c>
+      <c r="E438" s="6">
+        <v>12</v>
+      </c>
+      <c r="F438" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" ht="13.55" customHeight="1">
+      <c r="A439" t="s" s="5">
+        <v>880</v>
+      </c>
+      <c r="B439" t="s" s="5">
+        <v>881</v>
+      </c>
+      <c r="C439" s="6">
+        <v>4</v>
+      </c>
+      <c r="D439" s="6">
+        <v>12</v>
+      </c>
+      <c r="E439" s="6">
+        <v>12</v>
+      </c>
+      <c r="F439" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" ht="13.55" customHeight="1">
+      <c r="A440" t="s" s="5">
+        <v>882</v>
+      </c>
+      <c r="B440" t="s" s="5">
+        <v>883</v>
+      </c>
+      <c r="C440" s="6">
+        <v>2</v>
+      </c>
+      <c r="D440" s="6">
+        <v>8</v>
+      </c>
+      <c r="E440" s="6">
+        <v>10</v>
+      </c>
+      <c r="F440" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" ht="13.55" customHeight="1">
+      <c r="A441" t="s" s="5">
+        <v>884</v>
+      </c>
+      <c r="B441" t="s" s="5">
+        <v>885</v>
+      </c>
+      <c r="C441" s="6">
+        <v>3</v>
+      </c>
+      <c r="D441" s="6">
+        <v>10</v>
+      </c>
+      <c r="E441" s="6">
+        <v>10</v>
+      </c>
+      <c r="F441" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" ht="13.55" customHeight="1">
+      <c r="A442" t="s" s="5">
+        <v>886</v>
+      </c>
+      <c r="B442" t="s" s="5">
+        <v>887</v>
+      </c>
+      <c r="C442" s="6">
+        <v>1</v>
+      </c>
+      <c r="D442" s="6">
+        <v>4</v>
+      </c>
+      <c r="E442" s="6">
+        <v>6</v>
+      </c>
+      <c r="F442" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" ht="13.55" customHeight="1">
+      <c r="A443" t="s" s="5">
+        <v>888</v>
+      </c>
+      <c r="B443" t="s" s="5">
+        <v>889</v>
+      </c>
+      <c r="C443" s="6">
+        <v>1</v>
+      </c>
+      <c r="D443" s="6">
+        <v>2</v>
+      </c>
+      <c r="E443" s="6">
+        <v>6</v>
+      </c>
+      <c r="F443" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new log data file for November 2024
Created a new CSV file, saved_df_2024_11.csv, to store log entries for November 2024. This file captures detailed timestamped events and machine configurations for troubleshooting and analysis purposes.
</commit_message>
<xml_diff>
--- a/data/tiempo_final.xlsx
+++ b/data/tiempo_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="910">
   <si>
     <t>timestamp</t>
   </si>
@@ -2681,6 +2681,66 @@
   </si>
   <si>
     <t>020216.NC</t>
+  </si>
+  <si>
+    <t>2024-11-04 13:26:13</t>
+  </si>
+  <si>
+    <t>020263.NC</t>
+  </si>
+  <si>
+    <t>2024-11-04 14:22:09</t>
+  </si>
+  <si>
+    <t>020236.NC</t>
+  </si>
+  <si>
+    <t>2024-11-04 16:10:12</t>
+  </si>
+  <si>
+    <t>020239.NC</t>
+  </si>
+  <si>
+    <t>2024-11-05 08:52:00</t>
+  </si>
+  <si>
+    <t>020238.NC</t>
+  </si>
+  <si>
+    <t>2024-11-05 10:01:15</t>
+  </si>
+  <si>
+    <t>020237.NC</t>
+  </si>
+  <si>
+    <t>2024-11-05 12:24:03</t>
+  </si>
+  <si>
+    <t>L_15430.NC</t>
+  </si>
+  <si>
+    <t>2024-11-05 14:01:46</t>
+  </si>
+  <si>
+    <t>L_15431.NC</t>
+  </si>
+  <si>
+    <t>2024-11-06 07:59:18</t>
+  </si>
+  <si>
+    <t>L_15433.NC</t>
+  </si>
+  <si>
+    <t>2024-11-06 10:22:03</t>
+  </si>
+  <si>
+    <t>L_15432.NC</t>
+  </si>
+  <si>
+    <t>2024-11-06 14:14:22</t>
+  </si>
+  <si>
+    <t>020084.NC</t>
   </si>
 </sst>
 </file>
@@ -3918,15 +3978,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F443"/>
+  <dimension ref="A1:F453"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.5859" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.9688" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="6" width="8.85156" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12787,6 +12845,206 @@
         <v>6</v>
       </c>
       <c r="F443" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" ht="13.55" customHeight="1">
+      <c r="A444" t="s" s="5">
+        <v>890</v>
+      </c>
+      <c r="B444" t="s" s="5">
+        <v>891</v>
+      </c>
+      <c r="C444" s="6">
+        <v>6</v>
+      </c>
+      <c r="D444" s="6">
+        <v>19</v>
+      </c>
+      <c r="E444" s="6">
+        <v>12</v>
+      </c>
+      <c r="F444" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" ht="13.55" customHeight="1">
+      <c r="A445" t="s" s="5">
+        <v>892</v>
+      </c>
+      <c r="B445" t="s" s="5">
+        <v>893</v>
+      </c>
+      <c r="C445" s="6">
+        <v>10</v>
+      </c>
+      <c r="D445" s="6">
+        <v>50</v>
+      </c>
+      <c r="E445" s="6">
+        <v>3</v>
+      </c>
+      <c r="F445" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" ht="13.55" customHeight="1">
+      <c r="A446" t="s" s="5">
+        <v>894</v>
+      </c>
+      <c r="B446" t="s" s="5">
+        <v>895</v>
+      </c>
+      <c r="C446" s="6">
+        <v>45</v>
+      </c>
+      <c r="D446" s="6">
+        <v>31</v>
+      </c>
+      <c r="E446" s="6">
+        <v>20</v>
+      </c>
+      <c r="F446" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" ht="13.55" customHeight="1">
+      <c r="A447" t="s" s="5">
+        <v>896</v>
+      </c>
+      <c r="B447" t="s" s="5">
+        <v>897</v>
+      </c>
+      <c r="C447" s="6">
+        <v>6</v>
+      </c>
+      <c r="D447" s="6">
+        <v>7</v>
+      </c>
+      <c r="E447" s="6">
+        <v>16</v>
+      </c>
+      <c r="F447" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" ht="13.55" customHeight="1">
+      <c r="A448" t="s" s="5">
+        <v>898</v>
+      </c>
+      <c r="B448" t="s" s="5">
+        <v>899</v>
+      </c>
+      <c r="C448" s="6">
+        <v>5</v>
+      </c>
+      <c r="D448" s="6">
+        <v>18</v>
+      </c>
+      <c r="E448" s="6">
+        <v>8</v>
+      </c>
+      <c r="F448" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" ht="13.55" customHeight="1">
+      <c r="A449" t="s" s="5">
+        <v>900</v>
+      </c>
+      <c r="B449" t="s" s="5">
+        <v>901</v>
+      </c>
+      <c r="C449" s="6">
+        <v>1</v>
+      </c>
+      <c r="D449" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="E449" s="6">
+        <v>8</v>
+      </c>
+      <c r="F449" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" ht="13.55" customHeight="1">
+      <c r="A450" t="s" s="5">
+        <v>902</v>
+      </c>
+      <c r="B450" t="s" s="5">
+        <v>903</v>
+      </c>
+      <c r="C450" s="6">
+        <v>5</v>
+      </c>
+      <c r="D450" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="E450" s="6">
+        <v>10</v>
+      </c>
+      <c r="F450" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" ht="13.55" customHeight="1">
+      <c r="A451" t="s" s="5">
+        <v>904</v>
+      </c>
+      <c r="B451" t="s" s="5">
+        <v>905</v>
+      </c>
+      <c r="C451" s="6">
+        <v>29</v>
+      </c>
+      <c r="D451" s="6">
+        <v>143</v>
+      </c>
+      <c r="E451" s="6">
+        <v>10</v>
+      </c>
+      <c r="F451" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" ht="13.55" customHeight="1">
+      <c r="A452" t="s" s="5">
+        <v>906</v>
+      </c>
+      <c r="B452" t="s" s="5">
+        <v>907</v>
+      </c>
+      <c r="C452" s="6">
+        <v>26</v>
+      </c>
+      <c r="D452" s="6">
+        <v>91</v>
+      </c>
+      <c r="E452" s="6">
+        <v>10</v>
+      </c>
+      <c r="F452" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" ht="13.55" customHeight="1">
+      <c r="A453" t="s" s="5">
+        <v>908</v>
+      </c>
+      <c r="B453" t="s" s="5">
+        <v>909</v>
+      </c>
+      <c r="C453" s="6">
+        <v>8</v>
+      </c>
+      <c r="D453" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="E453" s="6">
+        <v>6</v>
+      </c>
+      <c r="F453" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refine data export formats for consistency
Standardize the formatting for data exports in the updated files to ensure uniformity in data handling across different spreadsheets and CSV files. This change enhances the compatibility of datasets for downstream analysis and reporting processes.
</commit_message>
<xml_diff>
--- a/data/tiempo_final.xlsx
+++ b/data/tiempo_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="982">
   <si>
     <t>timestamp</t>
   </si>
@@ -2741,6 +2741,222 @@
   </si>
   <si>
     <t>020084.NC</t>
+  </si>
+  <si>
+    <t>2024-11-07 09:50:44</t>
+  </si>
+  <si>
+    <t>020071.NC</t>
+  </si>
+  <si>
+    <t>2024-11-11 15:54:01</t>
+  </si>
+  <si>
+    <t>020146.NC</t>
+  </si>
+  <si>
+    <t>2024-11-12 14:14:47</t>
+  </si>
+  <si>
+    <t>020090.slp</t>
+  </si>
+  <si>
+    <t>2024-11-13 11:37:59</t>
+  </si>
+  <si>
+    <t>020249.NC</t>
+  </si>
+  <si>
+    <t>2024-11-13 12:25:13</t>
+  </si>
+  <si>
+    <t>020275.NC</t>
+  </si>
+  <si>
+    <t>2024-11-13 13:30:47</t>
+  </si>
+  <si>
+    <t>020272.NC</t>
+  </si>
+  <si>
+    <t>2024-11-14 10:02:01</t>
+  </si>
+  <si>
+    <t>020314.NC</t>
+  </si>
+  <si>
+    <t>2024-11-14 10:14:23</t>
+  </si>
+  <si>
+    <t>020289.NC</t>
+  </si>
+  <si>
+    <t>2024-11-14 15:42:03</t>
+  </si>
+  <si>
+    <t>020360.NC</t>
+  </si>
+  <si>
+    <t>2024-11-14 15:52:34</t>
+  </si>
+  <si>
+    <t>020345.NC</t>
+  </si>
+  <si>
+    <t>2024-11-18 15:32:28</t>
+  </si>
+  <si>
+    <t>020521.NC</t>
+  </si>
+  <si>
+    <t>2024-11-19 13:26:14</t>
+  </si>
+  <si>
+    <t>020507.NC</t>
+  </si>
+  <si>
+    <t>2024-11-20 07:54:21</t>
+  </si>
+  <si>
+    <t>020496.NC</t>
+  </si>
+  <si>
+    <t>2024-11-20 11:43:15</t>
+  </si>
+  <si>
+    <t>020505.NC</t>
+  </si>
+  <si>
+    <t>2024-11-20 14:37:55</t>
+  </si>
+  <si>
+    <t>020503.NC</t>
+  </si>
+  <si>
+    <t>2024-11-07 11:06:01</t>
+  </si>
+  <si>
+    <t>020105.NC</t>
+  </si>
+  <si>
+    <t>2024-11-20 17:27:26</t>
+  </si>
+  <si>
+    <t>020501.NC</t>
+  </si>
+  <si>
+    <t>2024-11-20 21:01:32</t>
+  </si>
+  <si>
+    <t>020908.NC</t>
+  </si>
+  <si>
+    <t>2024-11-21 19:57:12</t>
+  </si>
+  <si>
+    <t>020509.NC</t>
+  </si>
+  <si>
+    <t>2024-11-22 02:47:57</t>
+  </si>
+  <si>
+    <t>020490.NC</t>
+  </si>
+  <si>
+    <t>2024-11-25 17:07:02</t>
+  </si>
+  <si>
+    <t>020508.NC</t>
+  </si>
+  <si>
+    <t>2024-11-25 21:08:54</t>
+  </si>
+  <si>
+    <t>020494.NC</t>
+  </si>
+  <si>
+    <t>2024-11-25 23:36:32</t>
+  </si>
+  <si>
+    <t>020917.NC</t>
+  </si>
+  <si>
+    <t>2024-11-26 15:57:14</t>
+  </si>
+  <si>
+    <t>020867.NC</t>
+  </si>
+  <si>
+    <t>2024-11-26 16:20:02</t>
+  </si>
+  <si>
+    <t>021137.NC</t>
+  </si>
+  <si>
+    <t>2024-11-26 16:59:00</t>
+  </si>
+  <si>
+    <t>021059.NC</t>
+  </si>
+  <si>
+    <t>2024-11-26 17:02:41</t>
+  </si>
+  <si>
+    <t>020870.NC</t>
+  </si>
+  <si>
+    <t>2024-11-26 19:49:30</t>
+  </si>
+  <si>
+    <t>020869.NC</t>
+  </si>
+  <si>
+    <t>2024-11-27 02:29:57</t>
+  </si>
+  <si>
+    <t>020909.NC</t>
+  </si>
+  <si>
+    <t>2024-11-28 03:38:50</t>
+  </si>
+  <si>
+    <t>021058.NC</t>
+  </si>
+  <si>
+    <t>2024-11-28 05:27:21</t>
+  </si>
+  <si>
+    <t>021057.NC</t>
+  </si>
+  <si>
+    <t>2024-11-28 09:25:12</t>
+  </si>
+  <si>
+    <t>021054.NC</t>
+  </si>
+  <si>
+    <t>2024-11-28 12:10:00</t>
+  </si>
+  <si>
+    <t>020030.NC</t>
+  </si>
+  <si>
+    <t>2024-11-28 15:43:19</t>
+  </si>
+  <si>
+    <t>021424.NC</t>
+  </si>
+  <si>
+    <t>2024-11-28 19:26:51</t>
+  </si>
+  <si>
+    <t>021425.NC</t>
+  </si>
+  <si>
+    <t>2024-11-28 22:48:20</t>
+  </si>
+  <si>
+    <t>020910.NC</t>
   </si>
 </sst>
 </file>
@@ -3978,13 +4194,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F453"/>
+  <dimension ref="A1:F489"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7812" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13045,6 +13263,726 @@
         <v>6</v>
       </c>
       <c r="F453" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" ht="13.55" customHeight="1">
+      <c r="A454" t="s" s="5">
+        <v>910</v>
+      </c>
+      <c r="B454" t="s" s="5">
+        <v>911</v>
+      </c>
+      <c r="C454" s="6">
+        <v>20</v>
+      </c>
+      <c r="D454" s="6">
+        <v>12</v>
+      </c>
+      <c r="E454" s="6">
+        <v>25</v>
+      </c>
+      <c r="F454" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" ht="13.55" customHeight="1">
+      <c r="A455" t="s" s="5">
+        <v>912</v>
+      </c>
+      <c r="B455" t="s" s="5">
+        <v>913</v>
+      </c>
+      <c r="C455" s="6">
+        <v>1</v>
+      </c>
+      <c r="D455" s="6">
+        <v>2</v>
+      </c>
+      <c r="E455" s="6">
+        <v>12</v>
+      </c>
+      <c r="F455" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" ht="13.55" customHeight="1">
+      <c r="A456" t="s" s="5">
+        <v>914</v>
+      </c>
+      <c r="B456" t="s" s="5">
+        <v>915</v>
+      </c>
+      <c r="C456" s="6">
+        <v>14</v>
+      </c>
+      <c r="D456" s="6">
+        <v>208</v>
+      </c>
+      <c r="E456" s="6">
+        <v>5</v>
+      </c>
+      <c r="F456" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" ht="13.55" customHeight="1">
+      <c r="A457" t="s" s="5">
+        <v>916</v>
+      </c>
+      <c r="B457" t="s" s="5">
+        <v>917</v>
+      </c>
+      <c r="C457" s="6">
+        <v>24</v>
+      </c>
+      <c r="D457" s="6">
+        <v>73</v>
+      </c>
+      <c r="E457" s="6">
+        <v>10</v>
+      </c>
+      <c r="F457" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" ht="13.55" customHeight="1">
+      <c r="A458" t="s" s="5">
+        <v>918</v>
+      </c>
+      <c r="B458" t="s" s="5">
+        <v>919</v>
+      </c>
+      <c r="C458" s="6">
+        <v>41</v>
+      </c>
+      <c r="D458" s="6">
+        <v>34</v>
+      </c>
+      <c r="E458" s="6">
+        <v>20</v>
+      </c>
+      <c r="F458" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" ht="13.55" customHeight="1">
+      <c r="A459" t="s" s="5">
+        <v>920</v>
+      </c>
+      <c r="B459" t="s" s="5">
+        <v>921</v>
+      </c>
+      <c r="C459" s="6">
+        <v>13</v>
+      </c>
+      <c r="D459" s="6">
+        <v>11</v>
+      </c>
+      <c r="E459" s="6">
+        <v>20</v>
+      </c>
+      <c r="F459" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" ht="13.55" customHeight="1">
+      <c r="A460" t="s" s="5">
+        <v>922</v>
+      </c>
+      <c r="B460" t="s" s="5">
+        <v>923</v>
+      </c>
+      <c r="C460" s="6">
+        <v>44</v>
+      </c>
+      <c r="D460" s="6">
+        <v>264</v>
+      </c>
+      <c r="E460" s="6">
+        <v>8</v>
+      </c>
+      <c r="F460" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" ht="13.55" customHeight="1">
+      <c r="A461" t="s" s="5">
+        <v>924</v>
+      </c>
+      <c r="B461" t="s" s="5">
+        <v>925</v>
+      </c>
+      <c r="C461" s="6">
+        <v>30</v>
+      </c>
+      <c r="D461" s="6">
+        <v>14</v>
+      </c>
+      <c r="E461" s="6">
+        <v>2</v>
+      </c>
+      <c r="F461" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" ht="13.55" customHeight="1">
+      <c r="A462" t="s" s="5">
+        <v>926</v>
+      </c>
+      <c r="B462" t="s" s="5">
+        <v>927</v>
+      </c>
+      <c r="C462" s="6">
+        <v>1</v>
+      </c>
+      <c r="D462" s="6">
+        <v>5</v>
+      </c>
+      <c r="E462" s="6">
+        <v>5</v>
+      </c>
+      <c r="F462" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" ht="13.55" customHeight="1">
+      <c r="A463" t="s" s="5">
+        <v>928</v>
+      </c>
+      <c r="B463" t="s" s="5">
+        <v>929</v>
+      </c>
+      <c r="C463" s="6">
+        <v>47</v>
+      </c>
+      <c r="D463" s="6">
+        <v>145</v>
+      </c>
+      <c r="E463" s="6">
+        <v>8</v>
+      </c>
+      <c r="F463" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" ht="13.55" customHeight="1">
+      <c r="A464" t="s" s="5">
+        <v>930</v>
+      </c>
+      <c r="B464" t="s" s="5">
+        <v>931</v>
+      </c>
+      <c r="C464" s="6">
+        <v>33</v>
+      </c>
+      <c r="D464" s="6">
+        <v>18</v>
+      </c>
+      <c r="E464" s="6">
+        <v>16</v>
+      </c>
+      <c r="F464" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" ht="13.55" customHeight="1">
+      <c r="A465" t="s" s="5">
+        <v>932</v>
+      </c>
+      <c r="B465" t="s" s="5">
+        <v>933</v>
+      </c>
+      <c r="C465" s="6">
+        <v>71</v>
+      </c>
+      <c r="D465" s="6">
+        <v>500</v>
+      </c>
+      <c r="E465" s="6">
+        <v>6</v>
+      </c>
+      <c r="F465" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" ht="13.55" customHeight="1">
+      <c r="A466" t="s" s="5">
+        <v>934</v>
+      </c>
+      <c r="B466" t="s" s="5">
+        <v>935</v>
+      </c>
+      <c r="C466" s="6">
+        <v>72</v>
+      </c>
+      <c r="D466" s="6">
+        <v>500</v>
+      </c>
+      <c r="E466" s="6">
+        <v>6</v>
+      </c>
+      <c r="F466" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" ht="13.55" customHeight="1">
+      <c r="A467" t="s" s="5">
+        <v>936</v>
+      </c>
+      <c r="B467" t="s" s="5">
+        <v>937</v>
+      </c>
+      <c r="C467" s="6">
+        <v>72</v>
+      </c>
+      <c r="D467" s="6">
+        <v>500</v>
+      </c>
+      <c r="E467" s="6">
+        <v>6</v>
+      </c>
+      <c r="F467" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" ht="13.55" customHeight="1">
+      <c r="A468" t="s" s="5">
+        <v>938</v>
+      </c>
+      <c r="B468" t="s" s="5">
+        <v>939</v>
+      </c>
+      <c r="C468" s="6">
+        <v>71</v>
+      </c>
+      <c r="D468" s="6">
+        <v>500</v>
+      </c>
+      <c r="E468" s="6">
+        <v>6</v>
+      </c>
+      <c r="F468" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" ht="13.55" customHeight="1">
+      <c r="A469" t="s" s="5">
+        <v>940</v>
+      </c>
+      <c r="B469" t="s" s="5">
+        <v>941</v>
+      </c>
+      <c r="C469" s="6">
+        <v>1116</v>
+      </c>
+      <c r="D469" s="6">
+        <v>824.4</v>
+      </c>
+      <c r="E469" s="6">
+        <v>25</v>
+      </c>
+      <c r="F469" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" ht="13.55" customHeight="1">
+      <c r="A470" t="s" s="5">
+        <v>942</v>
+      </c>
+      <c r="B470" t="s" s="5">
+        <v>943</v>
+      </c>
+      <c r="C470" s="6">
+        <v>72</v>
+      </c>
+      <c r="D470" s="6">
+        <v>500</v>
+      </c>
+      <c r="E470" s="6">
+        <v>6</v>
+      </c>
+      <c r="F470" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" ht="13.55" customHeight="1">
+      <c r="A471" t="s" s="5">
+        <v>944</v>
+      </c>
+      <c r="B471" t="s" s="5">
+        <v>945</v>
+      </c>
+      <c r="C471" s="6">
+        <v>576</v>
+      </c>
+      <c r="D471" s="6">
+        <v>158</v>
+      </c>
+      <c r="E471" s="6">
+        <v>32</v>
+      </c>
+      <c r="F471" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" ht="13.55" customHeight="1">
+      <c r="A472" t="s" s="5">
+        <v>946</v>
+      </c>
+      <c r="B472" t="s" s="5">
+        <v>947</v>
+      </c>
+      <c r="C472" s="6">
+        <v>86</v>
+      </c>
+      <c r="D472" s="6">
+        <v>594</v>
+      </c>
+      <c r="E472" s="6">
+        <v>6</v>
+      </c>
+      <c r="F472" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" ht="13.55" customHeight="1">
+      <c r="A473" t="s" s="5">
+        <v>948</v>
+      </c>
+      <c r="B473" t="s" s="5">
+        <v>949</v>
+      </c>
+      <c r="C473" s="6">
+        <v>71</v>
+      </c>
+      <c r="D473" s="6">
+        <v>500</v>
+      </c>
+      <c r="E473" s="6">
+        <v>6</v>
+      </c>
+      <c r="F473" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" ht="13.55" customHeight="1">
+      <c r="A474" t="s" s="5">
+        <v>950</v>
+      </c>
+      <c r="B474" t="s" s="5">
+        <v>951</v>
+      </c>
+      <c r="C474" s="6">
+        <v>78</v>
+      </c>
+      <c r="D474" s="6">
+        <v>529</v>
+      </c>
+      <c r="E474" s="6">
+        <v>6</v>
+      </c>
+      <c r="F474" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" ht="13.55" customHeight="1">
+      <c r="A475" t="s" s="5">
+        <v>952</v>
+      </c>
+      <c r="B475" t="s" s="5">
+        <v>953</v>
+      </c>
+      <c r="C475" s="6">
+        <v>77</v>
+      </c>
+      <c r="D475" s="6">
+        <v>529</v>
+      </c>
+      <c r="E475" s="6">
+        <v>6</v>
+      </c>
+      <c r="F475" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" ht="13.55" customHeight="1">
+      <c r="A476" t="s" s="5">
+        <v>954</v>
+      </c>
+      <c r="B476" t="s" s="5">
+        <v>955</v>
+      </c>
+      <c r="C476" s="6">
+        <v>661</v>
+      </c>
+      <c r="D476" s="6">
+        <v>207</v>
+      </c>
+      <c r="E476" s="6">
+        <v>32</v>
+      </c>
+      <c r="F476" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" ht="13.55" customHeight="1">
+      <c r="A477" t="s" s="5">
+        <v>956</v>
+      </c>
+      <c r="B477" t="s" s="5">
+        <v>957</v>
+      </c>
+      <c r="C477" s="6">
+        <v>16</v>
+      </c>
+      <c r="D477" s="6">
+        <v>133</v>
+      </c>
+      <c r="E477" s="6">
+        <v>6</v>
+      </c>
+      <c r="F477" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" ht="13.55" customHeight="1">
+      <c r="A478" t="s" s="5">
+        <v>958</v>
+      </c>
+      <c r="B478" t="s" s="5">
+        <v>959</v>
+      </c>
+      <c r="C478" s="6">
+        <v>3</v>
+      </c>
+      <c r="D478" s="6">
+        <v>12</v>
+      </c>
+      <c r="E478" s="6">
+        <v>6</v>
+      </c>
+      <c r="F478" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" ht="13.55" customHeight="1">
+      <c r="A479" t="s" s="5">
+        <v>960</v>
+      </c>
+      <c r="B479" t="s" s="5">
+        <v>961</v>
+      </c>
+      <c r="C479" s="6">
+        <v>9</v>
+      </c>
+      <c r="D479" s="6">
+        <v>35</v>
+      </c>
+      <c r="E479" s="6">
+        <v>6</v>
+      </c>
+      <c r="F479" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" ht="13.55" customHeight="1">
+      <c r="A480" t="s" s="5">
+        <v>962</v>
+      </c>
+      <c r="B480" t="s" s="5">
+        <v>963</v>
+      </c>
+      <c r="C480" s="6">
+        <v>30</v>
+      </c>
+      <c r="D480" s="6">
+        <v>122</v>
+      </c>
+      <c r="E480" s="6">
+        <v>10</v>
+      </c>
+      <c r="F480" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" ht="13.55" customHeight="1">
+      <c r="A481" t="s" s="5">
+        <v>964</v>
+      </c>
+      <c r="B481" t="s" s="5">
+        <v>965</v>
+      </c>
+      <c r="C481" s="6">
+        <v>79</v>
+      </c>
+      <c r="D481" s="6">
+        <v>385</v>
+      </c>
+      <c r="E481" s="6">
+        <v>10</v>
+      </c>
+      <c r="F481" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" ht="13.55" customHeight="1">
+      <c r="A482" t="s" s="5">
+        <v>966</v>
+      </c>
+      <c r="B482" t="s" s="5">
+        <v>967</v>
+      </c>
+      <c r="C482" s="6">
+        <v>506</v>
+      </c>
+      <c r="D482" s="6">
+        <v>155</v>
+      </c>
+      <c r="E482" s="6">
+        <v>32</v>
+      </c>
+      <c r="F482" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" ht="13.55" customHeight="1">
+      <c r="A483" t="s" s="5">
+        <v>968</v>
+      </c>
+      <c r="B483" t="s" s="5">
+        <v>969</v>
+      </c>
+      <c r="C483" s="6">
+        <v>24</v>
+      </c>
+      <c r="D483" s="6">
+        <v>122</v>
+      </c>
+      <c r="E483" s="6">
+        <v>6</v>
+      </c>
+      <c r="F483" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" ht="13.55" customHeight="1">
+      <c r="A484" t="s" s="5">
+        <v>970</v>
+      </c>
+      <c r="B484" t="s" s="5">
+        <v>971</v>
+      </c>
+      <c r="C484" s="6">
+        <v>24</v>
+      </c>
+      <c r="D484" s="6">
+        <v>122</v>
+      </c>
+      <c r="E484" s="6">
+        <v>6</v>
+      </c>
+      <c r="F484" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" ht="13.55" customHeight="1">
+      <c r="A485" t="s" s="5">
+        <v>972</v>
+      </c>
+      <c r="B485" t="s" s="5">
+        <v>973</v>
+      </c>
+      <c r="C485" s="6">
+        <v>55</v>
+      </c>
+      <c r="D485" s="6">
+        <v>257</v>
+      </c>
+      <c r="E485" s="6">
+        <v>6</v>
+      </c>
+      <c r="F485" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" ht="13.55" customHeight="1">
+      <c r="A486" t="s" s="5">
+        <v>974</v>
+      </c>
+      <c r="B486" t="s" s="5">
+        <v>975</v>
+      </c>
+      <c r="C486" s="6">
+        <v>41</v>
+      </c>
+      <c r="D486" s="6">
+        <v>195</v>
+      </c>
+      <c r="E486" s="6">
+        <v>6</v>
+      </c>
+      <c r="F486" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" ht="13.55" customHeight="1">
+      <c r="A487" t="s" s="5">
+        <v>976</v>
+      </c>
+      <c r="B487" t="s" s="5">
+        <v>977</v>
+      </c>
+      <c r="C487" s="6">
+        <v>99</v>
+      </c>
+      <c r="D487" s="6">
+        <v>466</v>
+      </c>
+      <c r="E487" s="6">
+        <v>6</v>
+      </c>
+      <c r="F487" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" ht="13.55" customHeight="1">
+      <c r="A488" t="s" s="5">
+        <v>978</v>
+      </c>
+      <c r="B488" t="s" s="5">
+        <v>979</v>
+      </c>
+      <c r="C488" s="6">
+        <v>49</v>
+      </c>
+      <c r="D488" s="6">
+        <v>242</v>
+      </c>
+      <c r="E488" s="6">
+        <v>6</v>
+      </c>
+      <c r="F488" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" ht="13.55" customHeight="1">
+      <c r="A489" t="s" s="5">
+        <v>980</v>
+      </c>
+      <c r="B489" t="s" s="5">
+        <v>981</v>
+      </c>
+      <c r="C489" s="6">
+        <v>673</v>
+      </c>
+      <c r="D489" s="6">
+        <v>177</v>
+      </c>
+      <c r="E489" s="6">
+        <v>32</v>
+      </c>
+      <c r="F489" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplify sidebar image rendering
Updated the sidebar image to use `use_container_width` for better responsiveness and improved layout consistency. Removed unused imports to streamline the code and reduce redundancy.
</commit_message>
<xml_diff>
--- a/data/tiempo_final.xlsx
+++ b/data/tiempo_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="992">
   <si>
     <t>timestamp</t>
   </si>
@@ -2957,6 +2957,36 @@
   </si>
   <si>
     <t>020910.NC</t>
+  </si>
+  <si>
+    <t>2024-11-21 01:17:43</t>
+  </si>
+  <si>
+    <t>020915.NC</t>
+  </si>
+  <si>
+    <t>2024-11-21 22:58:51</t>
+  </si>
+  <si>
+    <t>020504.NC</t>
+  </si>
+  <si>
+    <t>2024-11-22 01:08:59</t>
+  </si>
+  <si>
+    <t>020502.NC</t>
+  </si>
+  <si>
+    <t>2024-11-22 04:53:45</t>
+  </si>
+  <si>
+    <t>020500.NC</t>
+  </si>
+  <si>
+    <t>2024-11-22 12:19:13</t>
+  </si>
+  <si>
+    <t>020916.NC</t>
   </si>
 </sst>
 </file>
@@ -4194,15 +4224,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F489"/>
+  <dimension ref="A1:F494"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7812" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="6" width="8.85156" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13314,7 +13342,7 @@
         <v>915</v>
       </c>
       <c r="C456" s="6">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D456" s="6">
         <v>208</v>
@@ -13983,6 +14011,106 @@
         <v>32</v>
       </c>
       <c r="F489" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" ht="13.55" customHeight="1">
+      <c r="A490" t="s" s="5">
+        <v>982</v>
+      </c>
+      <c r="B490" t="s" s="5">
+        <v>983</v>
+      </c>
+      <c r="C490" s="6">
+        <v>269</v>
+      </c>
+      <c r="D490" s="6">
+        <v>202</v>
+      </c>
+      <c r="E490" s="6">
+        <v>32</v>
+      </c>
+      <c r="F490" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" ht="13.55" customHeight="1">
+      <c r="A491" t="s" s="5">
+        <v>984</v>
+      </c>
+      <c r="B491" t="s" s="5">
+        <v>985</v>
+      </c>
+      <c r="C491" s="6">
+        <v>76</v>
+      </c>
+      <c r="D491" s="6">
+        <v>500</v>
+      </c>
+      <c r="E491" s="6">
+        <v>6</v>
+      </c>
+      <c r="F491" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" ht="13.55" customHeight="1">
+      <c r="A492" t="s" s="5">
+        <v>986</v>
+      </c>
+      <c r="B492" t="s" s="5">
+        <v>987</v>
+      </c>
+      <c r="C492" s="6">
+        <v>66</v>
+      </c>
+      <c r="D492" s="6">
+        <v>500</v>
+      </c>
+      <c r="E492" s="6">
+        <v>6</v>
+      </c>
+      <c r="F492" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" ht="13.55" customHeight="1">
+      <c r="A493" t="s" s="5">
+        <v>988</v>
+      </c>
+      <c r="B493" t="s" s="5">
+        <v>989</v>
+      </c>
+      <c r="C493" s="6">
+        <v>71</v>
+      </c>
+      <c r="D493" s="6">
+        <v>500</v>
+      </c>
+      <c r="E493" s="6">
+        <v>6</v>
+      </c>
+      <c r="F493" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" ht="13.55" customHeight="1">
+      <c r="A494" t="s" s="5">
+        <v>990</v>
+      </c>
+      <c r="B494" t="s" s="5">
+        <v>991</v>
+      </c>
+      <c r="C494" s="6">
+        <v>630</v>
+      </c>
+      <c r="D494" s="6">
+        <v>199</v>
+      </c>
+      <c r="E494" s="6">
+        <v>32</v>
+      </c>
+      <c r="F494" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files and adjust sidebar image in app.py
Added a new CSV file and modified two existing Excel files with updated data. Updated the Streamlit sidebar image call to remove the `use_container_width` argument for better layout control.
</commit_message>
<xml_diff>
--- a/data/tiempo_final.xlsx
+++ b/data/tiempo_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1044">
   <si>
     <t>timestamp</t>
   </si>
@@ -2987,6 +2987,162 @@
   </si>
   <si>
     <t>020916.NC</t>
+  </si>
+  <si>
+    <t>2024-12-02 01:14:20</t>
+  </si>
+  <si>
+    <t>021267.NC</t>
+  </si>
+  <si>
+    <t>2024-12-03 08:57:56</t>
+  </si>
+  <si>
+    <t>21455.NC</t>
+  </si>
+  <si>
+    <t>2024-12-03 09:51:02</t>
+  </si>
+  <si>
+    <t>021461.NC</t>
+  </si>
+  <si>
+    <t>2024-12-03 10:22:09</t>
+  </si>
+  <si>
+    <t>021499.NC</t>
+  </si>
+  <si>
+    <t>2024-12-04 15:13:47</t>
+  </si>
+  <si>
+    <t>021522.NC</t>
+  </si>
+  <si>
+    <t>2024-12-04 16:38:03</t>
+  </si>
+  <si>
+    <t>021547.NC</t>
+  </si>
+  <si>
+    <t>2024-12-04 17:41:04</t>
+  </si>
+  <si>
+    <t>020922.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 10:52:40</t>
+  </si>
+  <si>
+    <t>021665.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 11:34:40</t>
+  </si>
+  <si>
+    <t>021666.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 12:30:07</t>
+  </si>
+  <si>
+    <t>021667.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 13:26:26</t>
+  </si>
+  <si>
+    <t>021670.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 14:11:46</t>
+  </si>
+  <si>
+    <t>021668.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 14:44:26</t>
+  </si>
+  <si>
+    <t>021669.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 15:47:17</t>
+  </si>
+  <si>
+    <t>020920.NC</t>
+  </si>
+  <si>
+    <t>2024-12-05 16:09:58</t>
+  </si>
+  <si>
+    <t>020919.NC</t>
+  </si>
+  <si>
+    <t>2024-12-06 08:06:34</t>
+  </si>
+  <si>
+    <t>020918.NC</t>
+  </si>
+  <si>
+    <t>2024-12-09 16:36:33</t>
+  </si>
+  <si>
+    <t>020921.NC</t>
+  </si>
+  <si>
+    <t>2024-12-10 11:10:49</t>
+  </si>
+  <si>
+    <t>020911.NC</t>
+  </si>
+  <si>
+    <t>2024-12-11 03:52:57</t>
+  </si>
+  <si>
+    <t>020912.NC</t>
+  </si>
+  <si>
+    <t>2024-12-12 00:45:31</t>
+  </si>
+  <si>
+    <t>021907.NC</t>
+  </si>
+  <si>
+    <t>2024-12-12 01:08:04</t>
+  </si>
+  <si>
+    <t>021825.NC</t>
+  </si>
+  <si>
+    <t>2024-12-12 02:23:21</t>
+  </si>
+  <si>
+    <t>020914.NC</t>
+  </si>
+  <si>
+    <t>2024-12-02 13:31:32</t>
+  </si>
+  <si>
+    <t>020923.NC</t>
+  </si>
+  <si>
+    <t>2024-12-03 08:46:46</t>
+  </si>
+  <si>
+    <t>021532.NC</t>
+  </si>
+  <si>
+    <t>2024-12-03 16:45:04</t>
+  </si>
+  <si>
+    <t>020924.NC</t>
+  </si>
+  <si>
+    <t>2024-12-04 08:57:31</t>
+  </si>
+  <si>
+    <t>020925.NC</t>
   </si>
 </sst>
 </file>
@@ -4224,13 +4380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F494"/>
+  <dimension ref="A1:F520"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.0391" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7734" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14111,6 +14269,526 @@
         <v>32</v>
       </c>
       <c r="F494" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" ht="13.55" customHeight="1">
+      <c r="A495" t="s" s="5">
+        <v>992</v>
+      </c>
+      <c r="B495" t="s" s="5">
+        <v>993</v>
+      </c>
+      <c r="C495" s="6">
+        <v>221</v>
+      </c>
+      <c r="D495" s="6">
+        <v>191</v>
+      </c>
+      <c r="E495" s="6">
+        <v>14</v>
+      </c>
+      <c r="F495" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" ht="13.55" customHeight="1">
+      <c r="A496" t="s" s="5">
+        <v>994</v>
+      </c>
+      <c r="B496" t="s" s="5">
+        <v>995</v>
+      </c>
+      <c r="C496" s="6">
+        <v>13</v>
+      </c>
+      <c r="D496" s="6">
+        <v>8</v>
+      </c>
+      <c r="E496" s="6">
+        <v>20</v>
+      </c>
+      <c r="F496" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497" ht="13.55" customHeight="1">
+      <c r="A497" t="s" s="5">
+        <v>996</v>
+      </c>
+      <c r="B497" t="s" s="5">
+        <v>997</v>
+      </c>
+      <c r="C497" s="6">
+        <v>9</v>
+      </c>
+      <c r="D497" s="6">
+        <v>4</v>
+      </c>
+      <c r="E497" s="6">
+        <v>25</v>
+      </c>
+      <c r="F497" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" ht="13.55" customHeight="1">
+      <c r="A498" t="s" s="5">
+        <v>998</v>
+      </c>
+      <c r="B498" t="s" s="5">
+        <v>999</v>
+      </c>
+      <c r="C498" s="6">
+        <v>20</v>
+      </c>
+      <c r="D498" s="6">
+        <v>127</v>
+      </c>
+      <c r="E498" s="6">
+        <v>20</v>
+      </c>
+      <c r="F498" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" ht="13.55" customHeight="1">
+      <c r="A499" t="s" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B499" t="s" s="5">
+        <v>1001</v>
+      </c>
+      <c r="C499" s="6">
+        <v>23</v>
+      </c>
+      <c r="D499" s="6">
+        <v>153</v>
+      </c>
+      <c r="E499" s="6">
+        <v>10</v>
+      </c>
+      <c r="F499" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" ht="13.55" customHeight="1">
+      <c r="A500" t="s" s="5">
+        <v>1002</v>
+      </c>
+      <c r="B500" t="s" s="5">
+        <v>1003</v>
+      </c>
+      <c r="C500" s="6">
+        <v>9</v>
+      </c>
+      <c r="D500" s="6">
+        <v>248</v>
+      </c>
+      <c r="E500" s="6">
+        <v>12</v>
+      </c>
+      <c r="F500" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" ht="13.55" customHeight="1">
+      <c r="A501" t="s" s="5">
+        <v>1004</v>
+      </c>
+      <c r="B501" t="s" s="5">
+        <v>1005</v>
+      </c>
+      <c r="C501" s="6">
+        <v>361</v>
+      </c>
+      <c r="D501" s="6">
+        <v>51</v>
+      </c>
+      <c r="E501" s="6">
+        <v>21</v>
+      </c>
+      <c r="F501" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" ht="13.55" customHeight="1">
+      <c r="A502" t="s" s="5">
+        <v>1006</v>
+      </c>
+      <c r="B502" t="s" s="5">
+        <v>1007</v>
+      </c>
+      <c r="C502" s="6">
+        <v>3</v>
+      </c>
+      <c r="D502" s="6">
+        <v>9</v>
+      </c>
+      <c r="E502" s="6">
+        <v>12</v>
+      </c>
+      <c r="F502" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" ht="13.55" customHeight="1">
+      <c r="A503" t="s" s="5">
+        <v>1008</v>
+      </c>
+      <c r="B503" t="s" s="5">
+        <v>1009</v>
+      </c>
+      <c r="C503" s="6">
+        <v>41</v>
+      </c>
+      <c r="D503" s="6">
+        <v>125</v>
+      </c>
+      <c r="E503" s="6">
+        <v>2</v>
+      </c>
+      <c r="F503" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504" ht="13.55" customHeight="1">
+      <c r="A504" t="s" s="5">
+        <v>1010</v>
+      </c>
+      <c r="B504" t="s" s="5">
+        <v>1011</v>
+      </c>
+      <c r="C504" s="6">
+        <v>44</v>
+      </c>
+      <c r="D504" s="6">
+        <v>125</v>
+      </c>
+      <c r="E504" s="6">
+        <v>2</v>
+      </c>
+      <c r="F504" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505" ht="13.55" customHeight="1">
+      <c r="A505" t="s" s="5">
+        <v>1012</v>
+      </c>
+      <c r="B505" t="s" s="5">
+        <v>1013</v>
+      </c>
+      <c r="C505" s="6">
+        <v>40</v>
+      </c>
+      <c r="D505" s="6">
+        <v>120</v>
+      </c>
+      <c r="E505" s="6">
+        <v>2</v>
+      </c>
+      <c r="F505" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506" ht="13.55" customHeight="1">
+      <c r="A506" t="s" s="5">
+        <v>1014</v>
+      </c>
+      <c r="B506" t="s" s="5">
+        <v>1015</v>
+      </c>
+      <c r="C506" s="6">
+        <v>20</v>
+      </c>
+      <c r="D506" s="6">
+        <v>88</v>
+      </c>
+      <c r="E506" s="6">
+        <v>2</v>
+      </c>
+      <c r="F506" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" ht="13.55" customHeight="1">
+      <c r="A507" t="s" s="5">
+        <v>1016</v>
+      </c>
+      <c r="B507" t="s" s="5">
+        <v>1017</v>
+      </c>
+      <c r="C507" s="6">
+        <v>11</v>
+      </c>
+      <c r="D507" s="6">
+        <v>36</v>
+      </c>
+      <c r="E507" s="6">
+        <v>2</v>
+      </c>
+      <c r="F507" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" ht="13.55" customHeight="1">
+      <c r="A508" t="s" s="5">
+        <v>1018</v>
+      </c>
+      <c r="B508" t="s" s="5">
+        <v>1019</v>
+      </c>
+      <c r="C508" s="6">
+        <v>596</v>
+      </c>
+      <c r="D508" s="6">
+        <v>183</v>
+      </c>
+      <c r="E508" s="6">
+        <v>32</v>
+      </c>
+      <c r="F508" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" ht="13.55" customHeight="1">
+      <c r="A509" t="s" s="5">
+        <v>1020</v>
+      </c>
+      <c r="B509" t="s" s="5">
+        <v>1021</v>
+      </c>
+      <c r="C509" s="6">
+        <v>559</v>
+      </c>
+      <c r="D509" s="6">
+        <v>167</v>
+      </c>
+      <c r="E509" s="6">
+        <v>32</v>
+      </c>
+      <c r="F509" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" ht="13.55" customHeight="1">
+      <c r="A510" t="s" s="5">
+        <v>1022</v>
+      </c>
+      <c r="B510" t="s" s="5">
+        <v>1023</v>
+      </c>
+      <c r="C510" s="6">
+        <v>398</v>
+      </c>
+      <c r="D510" s="6">
+        <v>195</v>
+      </c>
+      <c r="E510" s="6">
+        <v>32</v>
+      </c>
+      <c r="F510" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" ht="13.55" customHeight="1">
+      <c r="A511" t="s" s="5">
+        <v>1024</v>
+      </c>
+      <c r="B511" t="s" s="5">
+        <v>1025</v>
+      </c>
+      <c r="C511" s="6">
+        <v>451</v>
+      </c>
+      <c r="D511" s="6">
+        <v>170</v>
+      </c>
+      <c r="E511" s="6">
+        <v>32</v>
+      </c>
+      <c r="F511" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" ht="13.55" customHeight="1">
+      <c r="A512" t="s" s="5">
+        <v>1026</v>
+      </c>
+      <c r="B512" t="s" s="5">
+        <v>1027</v>
+      </c>
+      <c r="C512" s="6">
+        <v>531</v>
+      </c>
+      <c r="D512" s="6">
+        <v>155</v>
+      </c>
+      <c r="E512" s="6">
+        <v>32</v>
+      </c>
+      <c r="F512" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" ht="13.55" customHeight="1">
+      <c r="A513" t="s" s="5">
+        <v>1028</v>
+      </c>
+      <c r="B513" t="s" s="5">
+        <v>1029</v>
+      </c>
+      <c r="C513" s="6">
+        <v>589</v>
+      </c>
+      <c r="D513" s="6">
+        <v>160</v>
+      </c>
+      <c r="E513" s="6">
+        <v>32</v>
+      </c>
+      <c r="F513" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" ht="13.55" customHeight="1">
+      <c r="A514" t="s" s="5">
+        <v>1030</v>
+      </c>
+      <c r="B514" t="s" s="5">
+        <v>1031</v>
+      </c>
+      <c r="C514" s="6">
+        <v>8</v>
+      </c>
+      <c r="D514" s="6">
+        <v>15</v>
+      </c>
+      <c r="E514" s="6">
+        <v>10</v>
+      </c>
+      <c r="F514" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" ht="13.55" customHeight="1">
+      <c r="A515" t="s" s="5">
+        <v>1032</v>
+      </c>
+      <c r="B515" t="s" s="5">
+        <v>1033</v>
+      </c>
+      <c r="C515" s="6">
+        <v>10</v>
+      </c>
+      <c r="D515" s="6">
+        <v>122</v>
+      </c>
+      <c r="E515" s="6">
+        <v>6</v>
+      </c>
+      <c r="F515" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" ht="13.55" customHeight="1">
+      <c r="A516" t="s" s="5">
+        <v>1034</v>
+      </c>
+      <c r="B516" t="s" s="5">
+        <v>1035</v>
+      </c>
+      <c r="C516" s="6">
+        <v>576</v>
+      </c>
+      <c r="D516" s="6">
+        <v>163</v>
+      </c>
+      <c r="E516" s="6">
+        <v>32</v>
+      </c>
+      <c r="F516" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" ht="13.55" customHeight="1">
+      <c r="A517" t="s" s="5">
+        <v>1036</v>
+      </c>
+      <c r="B517" t="s" s="5">
+        <v>1037</v>
+      </c>
+      <c r="C517" s="6">
+        <v>616</v>
+      </c>
+      <c r="D517" s="6">
+        <v>170</v>
+      </c>
+      <c r="E517" s="6">
+        <v>38</v>
+      </c>
+      <c r="F517" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" ht="13.55" customHeight="1">
+      <c r="A518" t="s" s="5">
+        <v>1038</v>
+      </c>
+      <c r="B518" t="s" s="5">
+        <v>1039</v>
+      </c>
+      <c r="C518" s="6">
+        <v>12</v>
+      </c>
+      <c r="D518" s="6">
+        <v>27</v>
+      </c>
+      <c r="E518" s="6">
+        <v>12</v>
+      </c>
+      <c r="F518" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519" ht="13.55" customHeight="1">
+      <c r="A519" t="s" s="5">
+        <v>1040</v>
+      </c>
+      <c r="B519" t="s" s="5">
+        <v>1041</v>
+      </c>
+      <c r="C519" s="6">
+        <v>559</v>
+      </c>
+      <c r="D519" s="6">
+        <v>155</v>
+      </c>
+      <c r="E519" s="6">
+        <v>38</v>
+      </c>
+      <c r="F519" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520" ht="13.55" customHeight="1">
+      <c r="A520" t="s" s="5">
+        <v>1042</v>
+      </c>
+      <c r="B520" t="s" s="5">
+        <v>1043</v>
+      </c>
+      <c r="C520" s="6">
+        <v>314</v>
+      </c>
+      <c r="D520" s="6">
+        <v>87</v>
+      </c>
+      <c r="E520" s="6">
+        <v>38</v>
+      </c>
+      <c r="F520" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files with new information
Modified one CSV file and two Excel files to reflect updated data. Ensured consistency across datasets for accurate processing and analysis.
</commit_message>
<xml_diff>
--- a/data/tiempo_final.xlsx
+++ b/data/tiempo_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1092">
   <si>
     <t>timestamp</t>
   </si>
@@ -3143,6 +3143,150 @@
   </si>
   <si>
     <t>020925.NC</t>
+  </si>
+  <si>
+    <t>2024-12-12 23:22:54</t>
+  </si>
+  <si>
+    <t>021862.NC</t>
+  </si>
+  <si>
+    <t>2024-12-17 09:50:32</t>
+  </si>
+  <si>
+    <t>022048.NC</t>
+  </si>
+  <si>
+    <t>2024-12-18 08:46:33</t>
+  </si>
+  <si>
+    <t>021978.NC</t>
+  </si>
+  <si>
+    <t>2024-12-18 11:55:54</t>
+  </si>
+  <si>
+    <t>021954.NC</t>
+  </si>
+  <si>
+    <t>2024-12-18 12:08:47</t>
+  </si>
+  <si>
+    <t>021955.NC</t>
+  </si>
+  <si>
+    <t>2024-12-18 12:34:39</t>
+  </si>
+  <si>
+    <t>021874.NC</t>
+  </si>
+  <si>
+    <t>2024-12-18 13:39:05</t>
+  </si>
+  <si>
+    <t>022061.NC</t>
+  </si>
+  <si>
+    <t>2024-12-18 15:39:58</t>
+  </si>
+  <si>
+    <t>022019.NC</t>
+  </si>
+  <si>
+    <t>2024-12-19 13:10:56</t>
+  </si>
+  <si>
+    <t>022020.NC</t>
+  </si>
+  <si>
+    <t>2024-12-19 16:50:33</t>
+  </si>
+  <si>
+    <t>022203.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 10:43:11</t>
+  </si>
+  <si>
+    <t>022087.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 11:47:17</t>
+  </si>
+  <si>
+    <t>022110.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 12:10:03</t>
+  </si>
+  <si>
+    <t>022123.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 12:26:12</t>
+  </si>
+  <si>
+    <t>022133.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 13:00:44</t>
+  </si>
+  <si>
+    <t>022095.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 13:17:21</t>
+  </si>
+  <si>
+    <t>022086.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 13:28:30</t>
+  </si>
+  <si>
+    <t>022094.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 13:49:34</t>
+  </si>
+  <si>
+    <t>022093.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 14:58:26</t>
+  </si>
+  <si>
+    <t>022089.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 15:12:20</t>
+  </si>
+  <si>
+    <t>022092.NC</t>
+  </si>
+  <si>
+    <t>2024-12-20 15:51:20</t>
+  </si>
+  <si>
+    <t>022090.NC</t>
+  </si>
+  <si>
+    <t>2024-12-23 09:20:09</t>
+  </si>
+  <si>
+    <t>022096.NC</t>
+  </si>
+  <si>
+    <t>2024-12-23 10:26:46</t>
+  </si>
+  <si>
+    <t>022135.NC</t>
+  </si>
+  <si>
+    <t>2024-12-23 10:35:17</t>
+  </si>
+  <si>
+    <t>022136.NC</t>
   </si>
 </sst>
 </file>
@@ -4380,15 +4524,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F520"/>
+  <dimension ref="A1:F544"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20.0391" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7734" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7734" style="1" customWidth="1"/>
+    <col min="2" max="6" width="8.85156" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14303,7 +14446,7 @@
         <v>13</v>
       </c>
       <c r="D496" s="6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E496" s="6">
         <v>20</v>
@@ -14340,7 +14483,7 @@
         <v>999</v>
       </c>
       <c r="C498" s="6">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="D498" s="6">
         <v>127</v>
@@ -14380,7 +14523,7 @@
         <v>1003</v>
       </c>
       <c r="C500" s="6">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="D500" s="6">
         <v>248</v>
@@ -14740,7 +14883,7 @@
         <v>1039</v>
       </c>
       <c r="C518" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D518" s="6">
         <v>27</v>
@@ -14789,6 +14932,486 @@
         <v>38</v>
       </c>
       <c r="F520" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" ht="13.55" customHeight="1">
+      <c r="A521" t="s" s="5">
+        <v>1044</v>
+      </c>
+      <c r="B521" t="s" s="5">
+        <v>1045</v>
+      </c>
+      <c r="C521" s="6">
+        <v>100</v>
+      </c>
+      <c r="D521" s="6">
+        <v>24</v>
+      </c>
+      <c r="E521" s="6">
+        <v>38</v>
+      </c>
+      <c r="F521" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" ht="13.55" customHeight="1">
+      <c r="A522" t="s" s="5">
+        <v>1046</v>
+      </c>
+      <c r="B522" t="s" s="5">
+        <v>1047</v>
+      </c>
+      <c r="C522" s="6">
+        <v>253</v>
+      </c>
+      <c r="D522" s="6">
+        <v>133</v>
+      </c>
+      <c r="E522" s="6">
+        <v>25</v>
+      </c>
+      <c r="F522" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" ht="13.55" customHeight="1">
+      <c r="A523" t="s" s="5">
+        <v>1048</v>
+      </c>
+      <c r="B523" t="s" s="5">
+        <v>1049</v>
+      </c>
+      <c r="C523" s="6">
+        <v>11</v>
+      </c>
+      <c r="D523" s="6">
+        <v>25</v>
+      </c>
+      <c r="E523" s="6">
+        <v>12</v>
+      </c>
+      <c r="F523" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" ht="13.55" customHeight="1">
+      <c r="A524" t="s" s="5">
+        <v>1050</v>
+      </c>
+      <c r="B524" t="s" s="5">
+        <v>1051</v>
+      </c>
+      <c r="C524" s="6">
+        <v>6</v>
+      </c>
+      <c r="D524" s="6">
+        <v>9</v>
+      </c>
+      <c r="E524" s="6">
+        <v>2</v>
+      </c>
+      <c r="F524" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" ht="13.55" customHeight="1">
+      <c r="A525" t="s" s="5">
+        <v>1052</v>
+      </c>
+      <c r="B525" t="s" s="5">
+        <v>1053</v>
+      </c>
+      <c r="C525" s="6">
+        <v>6</v>
+      </c>
+      <c r="D525" s="6">
+        <v>9</v>
+      </c>
+      <c r="E525" s="6">
+        <v>2</v>
+      </c>
+      <c r="F525" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526" ht="13.55" customHeight="1">
+      <c r="A526" t="s" s="5">
+        <v>1054</v>
+      </c>
+      <c r="B526" t="s" s="5">
+        <v>1055</v>
+      </c>
+      <c r="C526" s="6">
+        <v>92</v>
+      </c>
+      <c r="D526" s="6">
+        <v>363</v>
+      </c>
+      <c r="E526" s="6">
+        <v>6</v>
+      </c>
+      <c r="F526" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" ht="13.55" customHeight="1">
+      <c r="A527" t="s" s="5">
+        <v>1056</v>
+      </c>
+      <c r="B527" t="s" s="5">
+        <v>1057</v>
+      </c>
+      <c r="C527" s="6">
+        <v>10</v>
+      </c>
+      <c r="D527" s="6">
+        <v>47</v>
+      </c>
+      <c r="E527" s="6">
+        <v>6</v>
+      </c>
+      <c r="F527" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" ht="13.55" customHeight="1">
+      <c r="A528" t="s" s="5">
+        <v>1058</v>
+      </c>
+      <c r="B528" t="s" s="5">
+        <v>1059</v>
+      </c>
+      <c r="C528" s="6">
+        <v>88</v>
+      </c>
+      <c r="D528" s="6">
+        <v>420</v>
+      </c>
+      <c r="E528" s="6">
+        <v>10</v>
+      </c>
+      <c r="F528" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" ht="13.55" customHeight="1">
+      <c r="A529" t="s" s="5">
+        <v>1060</v>
+      </c>
+      <c r="B529" t="s" s="5">
+        <v>1061</v>
+      </c>
+      <c r="C529" s="6">
+        <v>16</v>
+      </c>
+      <c r="D529" s="6">
+        <v>56</v>
+      </c>
+      <c r="E529" s="6">
+        <v>10</v>
+      </c>
+      <c r="F529" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="530" ht="13.55" customHeight="1">
+      <c r="A530" t="s" s="5">
+        <v>1062</v>
+      </c>
+      <c r="B530" t="s" s="5">
+        <v>1063</v>
+      </c>
+      <c r="C530" s="6">
+        <v>2</v>
+      </c>
+      <c r="D530" s="6">
+        <v>10</v>
+      </c>
+      <c r="E530" s="6">
+        <v>6</v>
+      </c>
+      <c r="F530" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531" ht="13.55" customHeight="1">
+      <c r="A531" t="s" s="5">
+        <v>1064</v>
+      </c>
+      <c r="B531" t="s" s="5">
+        <v>1065</v>
+      </c>
+      <c r="C531" s="6">
+        <v>3</v>
+      </c>
+      <c r="D531" s="6">
+        <v>17</v>
+      </c>
+      <c r="E531" s="6">
+        <v>2</v>
+      </c>
+      <c r="F531" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" ht="13.55" customHeight="1">
+      <c r="A532" t="s" s="5">
+        <v>1066</v>
+      </c>
+      <c r="B532" t="s" s="5">
+        <v>1067</v>
+      </c>
+      <c r="C532" s="6">
+        <v>2</v>
+      </c>
+      <c r="D532" s="6">
+        <v>7</v>
+      </c>
+      <c r="E532" s="6">
+        <v>2</v>
+      </c>
+      <c r="F532" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="533" ht="13.55" customHeight="1">
+      <c r="A533" t="s" s="5">
+        <v>1068</v>
+      </c>
+      <c r="B533" t="s" s="5">
+        <v>1069</v>
+      </c>
+      <c r="C533" s="6">
+        <v>1</v>
+      </c>
+      <c r="D533" s="6">
+        <v>6</v>
+      </c>
+      <c r="E533" s="6">
+        <v>2</v>
+      </c>
+      <c r="F533" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="534" ht="13.55" customHeight="1">
+      <c r="A534" t="s" s="5">
+        <v>1070</v>
+      </c>
+      <c r="B534" t="s" s="5">
+        <v>1071</v>
+      </c>
+      <c r="C534" s="6">
+        <v>1</v>
+      </c>
+      <c r="D534" s="6">
+        <v>11</v>
+      </c>
+      <c r="E534" s="6">
+        <v>2</v>
+      </c>
+      <c r="F534" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" ht="13.55" customHeight="1">
+      <c r="A535" t="s" s="5">
+        <v>1072</v>
+      </c>
+      <c r="B535" t="s" s="5">
+        <v>1073</v>
+      </c>
+      <c r="C535" s="6">
+        <v>2</v>
+      </c>
+      <c r="D535" s="6">
+        <v>17</v>
+      </c>
+      <c r="E535" s="6">
+        <v>2</v>
+      </c>
+      <c r="F535" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536" ht="13.55" customHeight="1">
+      <c r="A536" t="s" s="5">
+        <v>1074</v>
+      </c>
+      <c r="B536" t="s" s="5">
+        <v>1075</v>
+      </c>
+      <c r="C536" s="6">
+        <v>2</v>
+      </c>
+      <c r="D536" s="6">
+        <v>17</v>
+      </c>
+      <c r="E536" s="6">
+        <v>2</v>
+      </c>
+      <c r="F536" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="537" ht="13.55" customHeight="1">
+      <c r="A537" t="s" s="5">
+        <v>1076</v>
+      </c>
+      <c r="B537" t="s" s="5">
+        <v>1077</v>
+      </c>
+      <c r="C537" s="6">
+        <v>3</v>
+      </c>
+      <c r="D537" s="6">
+        <v>17</v>
+      </c>
+      <c r="E537" s="6">
+        <v>2</v>
+      </c>
+      <c r="F537" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538" ht="13.55" customHeight="1">
+      <c r="A538" t="s" s="5">
+        <v>1078</v>
+      </c>
+      <c r="B538" t="s" s="5">
+        <v>1079</v>
+      </c>
+      <c r="C538" s="6">
+        <v>1</v>
+      </c>
+      <c r="D538" s="6">
+        <v>17</v>
+      </c>
+      <c r="E538" s="6">
+        <v>2</v>
+      </c>
+      <c r="F538" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="539" ht="13.55" customHeight="1">
+      <c r="A539" t="s" s="5">
+        <v>1080</v>
+      </c>
+      <c r="B539" t="s" s="5">
+        <v>1081</v>
+      </c>
+      <c r="C539" s="6">
+        <v>3</v>
+      </c>
+      <c r="D539" s="6">
+        <v>17</v>
+      </c>
+      <c r="E539" s="6">
+        <v>2</v>
+      </c>
+      <c r="F539" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="540" ht="13.55" customHeight="1">
+      <c r="A540" t="s" s="5">
+        <v>1082</v>
+      </c>
+      <c r="B540" t="s" s="5">
+        <v>1083</v>
+      </c>
+      <c r="C540" s="6">
+        <v>4</v>
+      </c>
+      <c r="D540" s="6">
+        <v>17</v>
+      </c>
+      <c r="E540" s="6">
+        <v>2</v>
+      </c>
+      <c r="F540" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" ht="13.55" customHeight="1">
+      <c r="A541" t="s" s="5">
+        <v>1084</v>
+      </c>
+      <c r="B541" t="s" s="5">
+        <v>1085</v>
+      </c>
+      <c r="C541" s="6">
+        <v>3</v>
+      </c>
+      <c r="D541" s="6">
+        <v>17</v>
+      </c>
+      <c r="E541" s="6">
+        <v>2</v>
+      </c>
+      <c r="F541" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="542" ht="13.55" customHeight="1">
+      <c r="A542" t="s" s="5">
+        <v>1086</v>
+      </c>
+      <c r="B542" t="s" s="5">
+        <v>1087</v>
+      </c>
+      <c r="C542" s="6">
+        <v>4</v>
+      </c>
+      <c r="D542" s="6">
+        <v>18</v>
+      </c>
+      <c r="E542" s="6">
+        <v>2</v>
+      </c>
+      <c r="F542" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="543" ht="13.55" customHeight="1">
+      <c r="A543" t="s" s="5">
+        <v>1088</v>
+      </c>
+      <c r="B543" t="s" s="5">
+        <v>1089</v>
+      </c>
+      <c r="C543" s="6">
+        <v>1</v>
+      </c>
+      <c r="D543" s="6">
+        <v>9</v>
+      </c>
+      <c r="E543" s="6">
+        <v>2</v>
+      </c>
+      <c r="F543" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" ht="13.55" customHeight="1">
+      <c r="A544" t="s" s="5">
+        <v>1090</v>
+      </c>
+      <c r="B544" t="s" s="5">
+        <v>1091</v>
+      </c>
+      <c r="C544" s="6">
+        <v>2</v>
+      </c>
+      <c r="D544" s="6">
+        <v>15</v>
+      </c>
+      <c r="E544" s="6">
+        <v>2</v>
+      </c>
+      <c r="F544" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>